<commit_message>
different minor fixes, templates fixed, grouping logic fixed, addAmount fn need refactor
</commit_message>
<xml_diff>
--- a/templates/Export_Storage_Agreement.xlsx
+++ b/templates/Export_Storage_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5238CE-663C-43F6-8300-DC7B1847C22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2DF742-BA24-44DB-BE5F-DEC18E3F8D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15796" activeTab="1" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
+    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Storage_Contract" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="135">
   <si>
     <t>KTI COMPANY LIMITED ( Korea, Busan) ,  here in after referred to as Contractor, represented by the President SE JI YOUNG on one part, and "Tikhrybcom Co., LTD", (Russia, Magadan), here in after referred to asCustomer, represented by the  Deputy General Director M.N. Kruzina, acting on the basis of the Charter, on the other part, have concluded this Supplementary Agreement on the following:</t>
   </si>
@@ -128,11 +128,6 @@
     <t xml:space="preserve">Получатель сертификатов / Certificates' Consignee </t>
   </si>
   <si>
-    <t xml:space="preserve">Количество, тн. /
-Quantity, mt. 
-</t>
-  </si>
-  <si>
     <t>2. The Goods will be delivered to Busan, Korea by the transport vessel m/v "Bukhta Asacha" no later than June 10, 2023</t>
   </si>
   <si>
@@ -319,9 +314,6 @@
     <t>Вид упаковки</t>
   </si>
   <si>
-    <t>Места / Количество</t>
-  </si>
-  <si>
     <t>Цена</t>
   </si>
   <si>
@@ -427,12 +419,6 @@
     <t>2. Товар будет доставлен в г. Пусан, Южная Корея транспортным судном ТР "Бухта Асача" не позднее 10.06.2023</t>
   </si>
   <si>
-    <t>3. Во всем остальном, что не предусмотрено настоящим дополнительным соглашением, стороны руководствуются условиями договора оказания услуг хранения № 344/33957322/0157 от  02.04.2018</t>
-  </si>
-  <si>
-    <t>4. Настоящее дополнительное соглашение вступает в силу с момента его подписания и является неотъемлемой частью договора оказания услуг хранения №  344/33957322/0157 от  02.04.2018</t>
-  </si>
-  <si>
     <t>5. Настоящее дополнительное соглашение составлено и подписано в двух подлинных экземплярах, имеющих одинаковую юридическую силу.</t>
   </si>
   <si>
@@ -457,26 +443,16 @@
     <t>ТР "Фрио Севастополис"</t>
   </si>
   <si>
-    <t xml:space="preserve">к договору оказания услуг хранения №  410/33957322/0190
-</t>
-  </si>
-  <si>
     <t>Магадан, от 10 июля 2019</t>
   </si>
   <si>
     <t>____________________________________________________________________________________</t>
   </si>
   <si>
-    <t>1 000 шт /</t>
-  </si>
-  <si>
     <t>MSC Молоки минтая мороженые</t>
   </si>
   <si>
     <t>1/ 22,5 КГ</t>
-  </si>
-  <si>
-    <t>426 шт /</t>
   </si>
   <si>
     <t>9,585 тн</t>
@@ -525,6 +501,30 @@
   </si>
   <si>
     <t>Non-MSC certified</t>
+  </si>
+  <si>
+    <t>1 000 /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество, тн. /
+Quantity, tn. 
+</t>
+  </si>
+  <si>
+    <t>Места  / Количество</t>
+  </si>
+  <si>
+    <t>1 000 мест /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">к контракту оказания услуг хранения №  410/33957322/0190
+</t>
+  </si>
+  <si>
+    <t>3. Во всем остальном, что не предусмотрено настоящим дополнительным соглашением, стороны руководствуются условиями контракта оказания услуг хранения № 344/33957322/0157 от  02.04.2018</t>
+  </si>
+  <si>
+    <t>4. Настоящее дополнительное соглашение вступает в силу с момента его подписания и является неотъемлемой частью контракта оказания услуг хранения №  344/33957322/0157 от  02.04.2018</t>
   </si>
 </sst>
 </file>
@@ -1048,6 +1048,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1140,24 +1152,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -1183,250 +1183,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1836,8 +1592,8 @@
   </sheetPr>
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
@@ -1868,11 +1624,11 @@
     <row r="1" spans="1:24" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="87"/>
       <c r="B1" s="85" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="2"/>
@@ -1895,11 +1651,11 @@
     <row r="2" spans="1:24" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="87"/>
       <c r="B2" s="78" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" s="78"/>
       <c r="D2" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E2" s="78"/>
       <c r="F2" s="2"/>
@@ -1922,11 +1678,11 @@
     <row r="3" spans="1:24" s="98" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="88"/>
       <c r="B3" s="79" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" s="79"/>
       <c r="D3" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E3" s="79"/>
       <c r="F3" s="90"/>
@@ -1971,14 +1727,14 @@
     </row>
     <row r="5" spans="1:24" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="87"/>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="104" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="105"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="108" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="109"/>
       <c r="F5" s="2"/>
       <c r="G5"/>
       <c r="H5"/>
@@ -2001,14 +1757,14 @@
     </row>
     <row r="6" spans="1:24" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="87"/>
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="105"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="108" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="109"/>
       <c r="F6" s="2"/>
       <c r="G6"/>
       <c r="H6"/>
@@ -2041,7 +1797,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="92" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7"/>
@@ -2065,17 +1821,17 @@
     </row>
     <row r="8" spans="1:24" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="87"/>
-      <c r="B8" s="132" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="132" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="132" t="s">
-        <v>132</v>
+      <c r="B8" s="101" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="101" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="101" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="101" t="s">
+        <v>125</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8"/>
@@ -2099,14 +1855,14 @@
     </row>
     <row r="9" spans="1:24" s="100" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="89"/>
-      <c r="B9" s="121" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="120"/>
-      <c r="D9" s="119" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="120"/>
+      <c r="B9" s="125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="124"/>
+      <c r="D9" s="123" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="124"/>
       <c r="F9" s="91"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -2128,14 +1884,14 @@
     </row>
     <row r="10" spans="1:24" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="87"/>
-      <c r="B10" s="106" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="104" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="105"/>
+      <c r="B10" s="110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="109"/>
+      <c r="D10" s="108" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="109"/>
       <c r="F10" s="2"/>
       <c r="H10"/>
       <c r="I10"/>
@@ -2157,14 +1913,14 @@
     </row>
     <row r="11" spans="1:24" ht="55.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="87"/>
-      <c r="B11" s="106" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="104" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="105"/>
+      <c r="B11" s="110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="109"/>
+      <c r="D11" s="108" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="109"/>
       <c r="F11" s="2"/>
       <c r="H11"/>
       <c r="I11"/>
@@ -2186,14 +1942,14 @@
     </row>
     <row r="12" spans="1:24" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="87"/>
-      <c r="B12" s="106" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="104" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="105"/>
+      <c r="B12" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="109"/>
+      <c r="D12" s="108" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="109"/>
       <c r="F12" s="2"/>
       <c r="H12"/>
       <c r="I12"/>
@@ -2215,14 +1971,14 @@
     </row>
     <row r="13" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="87"/>
-      <c r="B13" s="113" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="114"/>
-      <c r="D13" s="113" t="s">
+      <c r="B13" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="114"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="118"/>
       <c r="F13" s="2"/>
       <c r="H13"/>
       <c r="I13"/>
@@ -2244,218 +2000,218 @@
     </row>
     <row r="14" spans="1:24" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="87"/>
-      <c r="B14" s="115" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="116"/>
-      <c r="D14" s="115" t="s">
+      <c r="B14" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="116"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="119" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="120"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="87"/>
-      <c r="B15" s="110" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="111"/>
-      <c r="D15" s="110" t="s">
+      <c r="B15" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="111"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="115"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="87"/>
-      <c r="B16" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="104" t="s">
+      <c r="B16" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="105"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="108" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="109"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="87"/>
-      <c r="B17" s="106" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="104" t="s">
+      <c r="B17" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="105"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="109"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="87"/>
-      <c r="B18" s="106" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="105"/>
-      <c r="D18" s="104" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="105"/>
+      <c r="B18" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="109"/>
+      <c r="D18" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="109"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="87"/>
-      <c r="B19" s="106" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="104" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="105"/>
+      <c r="B19" s="110" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="109"/>
+      <c r="D19" s="108" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="109"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="87"/>
-      <c r="B20" s="106" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="104" t="s">
+      <c r="B20" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="105"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="108" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="109"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="87"/>
-      <c r="B21" s="106" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="104" t="s">
+      <c r="B21" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="105"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="108" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="109"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="87"/>
-      <c r="B22" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="111"/>
-      <c r="D22" s="110" t="s">
+      <c r="B22" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="111"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="114" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="115"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="87"/>
-      <c r="B23" s="112" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="111"/>
-      <c r="D23" s="110" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="111"/>
+      <c r="B23" s="116" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="115"/>
+      <c r="D23" s="114" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="115"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="87"/>
-      <c r="B24" s="106" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="105"/>
-      <c r="D24" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="105"/>
+      <c r="B24" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="109"/>
+      <c r="D24" s="108" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="109"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="87"/>
-      <c r="B25" s="106" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="105"/>
-      <c r="D25" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="105"/>
+      <c r="B25" s="110" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="109"/>
+      <c r="D25" s="108" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="109"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="87"/>
-      <c r="B26" s="109" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="108"/>
-      <c r="D26" s="107" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="108"/>
+      <c r="B26" s="113" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="112"/>
+      <c r="D26" s="111" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="112"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="87"/>
-      <c r="B27" s="109" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="108"/>
-      <c r="D27" s="107" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="108"/>
+      <c r="B27" s="113" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="112"/>
+      <c r="D27" s="111" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="112"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="87"/>
-      <c r="B28" s="106" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="105"/>
-      <c r="D28" s="104" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="105"/>
+      <c r="B28" s="110" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="109"/>
+      <c r="D28" s="108" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="109"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="87"/>
-      <c r="B29" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="105"/>
-      <c r="D29" s="104" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="105"/>
+      <c r="B29" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="109"/>
+      <c r="D29" s="108" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="109"/>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="87"/>
-      <c r="B30" s="106" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="105"/>
-      <c r="D30" s="104" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="105"/>
+      <c r="B30" s="110" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="109"/>
+      <c r="D30" s="108" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="109"/>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="42.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="87"/>
-      <c r="B31" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="102"/>
-      <c r="D31" s="101" t="s">
+      <c r="B31" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="102"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="106"/>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -2528,32 +2284,32 @@
     <mergeCell ref="B30:C30"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:C7">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="21">
       <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:C7">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="24">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="24">
       <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="17">
       <formula>LEN(TRIM(D7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="18">
       <formula>LEN(TRIM(D7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="13">
       <formula>LEN(TRIM(E7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="14">
       <formula>LEN(TRIM(E7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2592,8 +2348,8 @@
   </sheetPr>
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView view="pageBreakPreview" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2613,7 +2369,7 @@
     <row r="1" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.85">
       <c r="B2" s="68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -2625,45 +2381,45 @@
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="103" t="s">
         <v>41</v>
-      </c>
-      <c r="H3" s="134" t="s">
-        <v>42</v>
       </c>
       <c r="I3" s="84"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="B4" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" s="133" t="s">
-        <v>76</v>
+        <v>127</v>
+      </c>
+      <c r="H4" s="102" t="s">
+        <v>74</v>
       </c>
       <c r="I4" s="84"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2675,13 +2431,13 @@
     </row>
     <row r="6" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="126" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="126"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -2691,12 +2447,12 @@
     <row r="7" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="B7" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="22"/>
       <c r="E7" s="20" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -2705,28 +2461,28 @@
     </row>
     <row r="8" spans="1:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
-      <c r="B8" s="124" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="124"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="126" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="128"/>
+      <c r="B8" s="128" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="128"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="130" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="132"/>
       <c r="I8" s="84"/>
     </row>
     <row r="9" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
       <c r="B9" s="80" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="57"/>
       <c r="D9" s="58"/>
       <c r="E9" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -2736,12 +2492,12 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
       <c r="B10" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="3"/>
       <c r="E10" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
@@ -2751,14 +2507,14 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="33" t="s">
         <v>47</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>48</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -2768,14 +2524,14 @@
     <row r="12" spans="1:9" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="81" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
@@ -2785,48 +2541,48 @@
     <row r="13" spans="1:9" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="D13" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="E13" s="36" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>52</v>
       </c>
       <c r="F13" s="36"/>
       <c r="G13" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="37" t="s">
         <v>53</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>54</v>
       </c>
       <c r="I13" s="84"/>
     </row>
     <row r="14" spans="1:9" ht="33.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="70" t="s">
+      <c r="E14" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="70" t="s">
-        <v>88</v>
-      </c>
       <c r="G14" s="70" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H14" s="71" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I14" s="84"/>
     </row>
@@ -2965,7 +2721,7 @@
     <row r="27" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="3"/>
       <c r="B27" s="73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="73"/>
       <c r="D27" s="73"/>
@@ -2978,7 +2734,7 @@
     <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
       <c r="B28" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -2991,7 +2747,7 @@
     <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
       <c r="B29" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
@@ -3004,7 +2760,7 @@
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -3019,17 +2775,17 @@
       <c r="B31" s="40"/>
       <c r="C31" s="41"/>
       <c r="D31" s="43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F31" s="43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G31" s="40"/>
       <c r="H31" s="74" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I31" s="84"/>
     </row>
@@ -3050,7 +2806,7 @@
       <c r="C33" s="49"/>
       <c r="D33" s="50"/>
       <c r="E33" s="51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -3221,7 +2977,7 @@
     </row>
     <row r="52" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.85">
       <c r="B52" s="68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" s="68"/>
       <c r="D52" s="68"/>
@@ -3233,45 +2989,45 @@
     <row r="53" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="3"/>
       <c r="B53" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="17"/>
       <c r="D53" s="19"/>
       <c r="E53" s="54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F53" s="55"/>
       <c r="G53" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" s="104" t="s">
         <v>41</v>
-      </c>
-      <c r="H53" s="135" t="s">
-        <v>42</v>
       </c>
       <c r="I53" s="84"/>
     </row>
     <row r="54" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="3"/>
       <c r="B54" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="22"/>
       <c r="E54" s="21" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H54" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I54" s="84"/>
     </row>
     <row r="55" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="3"/>
       <c r="B55" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C55" s="24"/>
       <c r="D55" s="25"/>
@@ -3284,12 +3040,12 @@
     <row r="56" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="3"/>
       <c r="B56" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="19"/>
       <c r="E56" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
@@ -3299,12 +3055,12 @@
     <row r="57" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="3"/>
       <c r="B57" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="22"/>
       <c r="E57" s="20" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F57" s="21"/>
       <c r="G57" s="21"/>
@@ -3313,28 +3069,28 @@
     </row>
     <row r="58" spans="1:9" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="3"/>
-      <c r="B58" s="129" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58" s="129"/>
-      <c r="D58" s="130"/>
-      <c r="E58" s="131" t="s">
-        <v>127</v>
-      </c>
-      <c r="F58" s="124"/>
-      <c r="G58" s="124"/>
-      <c r="H58" s="125"/>
+      <c r="B58" s="133" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="133"/>
+      <c r="D58" s="134"/>
+      <c r="E58" s="135" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" s="128"/>
+      <c r="G58" s="128"/>
+      <c r="H58" s="129"/>
       <c r="I58" s="84"/>
     </row>
     <row r="59" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="3"/>
       <c r="B59" s="80" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C59" s="57"/>
       <c r="D59" s="58"/>
       <c r="E59" s="59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F59" s="28"/>
       <c r="G59" s="28"/>
@@ -3344,12 +3100,12 @@
     <row r="60" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="3"/>
       <c r="B60" s="83" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C60" s="30"/>
       <c r="D60" s="3"/>
       <c r="E60" s="60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F60" s="61"/>
       <c r="G60" s="61"/>
@@ -3359,14 +3115,14 @@
     <row r="61" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="3"/>
       <c r="B61" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D61" s="34"/>
       <c r="E61" s="20" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="F61" s="21"/>
       <c r="G61" s="21"/>
@@ -3376,14 +3132,14 @@
     <row r="62" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="3"/>
       <c r="B62" s="47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="23" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F62" s="63"/>
       <c r="G62" s="63"/>
@@ -3393,48 +3149,48 @@
     <row r="63" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="3"/>
       <c r="B63" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C63" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="D63" s="65" t="s">
-        <v>67</v>
-      </c>
       <c r="E63" s="36" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="F63" s="36"/>
       <c r="G63" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H63" s="66" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I63" s="84"/>
     </row>
     <row r="64" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="3"/>
       <c r="B64" s="69" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C64" s="69" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D64" s="69" t="s">
-        <v>119</v>
-      </c>
-      <c r="E64" s="69" t="s">
-        <v>120</v>
+        <v>113</v>
+      </c>
+      <c r="E64" s="69">
+        <v>426</v>
       </c>
       <c r="F64" s="69" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G64" s="69" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H64" s="75" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="I64" s="84"/>
     </row>
@@ -3562,7 +3318,7 @@
     <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="3"/>
       <c r="B76" s="77" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C76" s="77"/>
       <c r="D76" s="77"/>
@@ -3575,7 +3331,7 @@
     <row r="77" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="3"/>
       <c r="B77" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -3588,7 +3344,7 @@
     <row r="78" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="3"/>
       <c r="B78" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
@@ -3601,7 +3357,7 @@
     <row r="79" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="3"/>
       <c r="B79" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -3616,16 +3372,16 @@
       <c r="B80" s="40"/>
       <c r="C80" s="41"/>
       <c r="D80" s="43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E80" s="42" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="F80" s="43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H80" s="42" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="I80" s="84"/>
     </row>
@@ -3646,7 +3402,7 @@
       <c r="C82" s="49"/>
       <c r="D82" s="50"/>
       <c r="E82" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>

</xml_diff>

<commit_message>
FCA beta ready, minor fixes contract added
</commit_message>
<xml_diff>
--- a/templates/Export_Storage_Agreement.xlsx
+++ b/templates/Export_Storage_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2DF742-BA24-44DB-BE5F-DEC18E3F8D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9701B6E0-7D63-4FCD-8C98-9BA078C3AE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Storage_Contract" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Storage_Contract!$A$1:$F$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Noncom_Invoice!$A$1:$I$92</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Noncom_Invoice!$A$1:$I$95</definedName>
     <definedName name="Адреса_банк_получателя">Export_Storage_Contract!$B$17</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Storage_Contract!$B$18</definedName>
     <definedName name="Адреса_банк_получателя_свифт">Export_Storage_Contract!$B$19</definedName>
@@ -39,49 +39,49 @@
     <definedName name="Доставка_транспорт">Export_Storage_Contract!$B$9</definedName>
     <definedName name="Инвойс">Noncom_Invoice!$E$4</definedName>
     <definedName name="Инвойс_Bl_массив">Noncom_Invoice!$B$14</definedName>
-    <definedName name="Инвойс_Bl_массив_п">Noncom_Invoice!$B$64</definedName>
+    <definedName name="Инвойс_Bl_массив_п">Noncom_Invoice!$B$67</definedName>
     <definedName name="Инвойс_контракт">Noncom_Invoice!$E$11</definedName>
     <definedName name="Инвойс_контракт_дата">Noncom_Invoice!$E$12</definedName>
-    <definedName name="Инвойс_контракт_дата_п">Noncom_Invoice!$E$62</definedName>
-    <definedName name="Инвойс_контракт_п">Noncom_Invoice!$E$61</definedName>
+    <definedName name="Инвойс_контракт_дата_п">Noncom_Invoice!$E$65</definedName>
+    <definedName name="Инвойс_контракт_п">Noncom_Invoice!$E$64</definedName>
     <definedName name="Инвойс_куда">Noncom_Invoice!$B$12</definedName>
-    <definedName name="Инвойс_куда_п">Noncom_Invoice!$B$62</definedName>
+    <definedName name="Инвойс_куда_п">Noncom_Invoice!$B$65</definedName>
     <definedName name="Инвойс_откуда">Noncom_Invoice!$C$12</definedName>
-    <definedName name="Инвойс_откуда_п">Noncom_Invoice!$C$62</definedName>
-    <definedName name="Инвойс_п">Noncom_Invoice!$E$54</definedName>
+    <definedName name="Инвойс_откуда_п">Noncom_Invoice!$C$65</definedName>
+    <definedName name="Инвойс_п">Noncom_Invoice!$E$57</definedName>
     <definedName name="Инвойс_подвал_всего">Noncom_Invoice!$F$31</definedName>
-    <definedName name="Инвойс_подвал_всего_п">Noncom_Invoice!$F$80</definedName>
+    <definedName name="Инвойс_подвал_всего_п">Noncom_Invoice!$F$83</definedName>
     <definedName name="Инвойс_подвал_места">Noncom_Invoice!$E$31</definedName>
-    <definedName name="Инвойс_подвал_места_п">Noncom_Invoice!$E$80</definedName>
+    <definedName name="Инвойс_подвал_места_п">Noncom_Invoice!$E$83</definedName>
     <definedName name="Инвойс_подвал_сумма">Noncom_Invoice!$H$31</definedName>
-    <definedName name="Инвойс_подвал_сумма_п">Noncom_Invoice!$H$80</definedName>
+    <definedName name="Инвойс_подвал_сумма_п">Noncom_Invoice!$H$83</definedName>
     <definedName name="Инвойс_подписант">Noncom_Invoice!$E$33</definedName>
-    <definedName name="Инвойс_подписант_п">Noncom_Invoice!$E$82</definedName>
+    <definedName name="Инвойс_подписант_п">Noncom_Invoice!$E$85</definedName>
     <definedName name="Инвойс_покупатель">Noncom_Invoice!$E$7</definedName>
     <definedName name="Инвойс_покупатель_адрес">Noncom_Invoice!$E$8</definedName>
-    <definedName name="Инвойс_покупатель_адрес_п">Noncom_Invoice!$E$58</definedName>
-    <definedName name="Инвойс_покупатель_п">Noncom_Invoice!$E$57</definedName>
+    <definedName name="Инвойс_покупатель_адрес_п">Noncom_Invoice!$E$61</definedName>
+    <definedName name="Инвойс_покупатель_п">Noncom_Invoice!$E$60</definedName>
     <definedName name="Инвойс_получатель">Noncom_Invoice!$B$7</definedName>
     <definedName name="Инвойс_получатель_адрес">Noncom_Invoice!$B$8</definedName>
-    <definedName name="Инвойс_получатель_адрес_п">Noncom_Invoice!$B$58</definedName>
-    <definedName name="Инвойс_получатель_п">Noncom_Invoice!$B$57</definedName>
+    <definedName name="Инвойс_получатель_адрес_п">Noncom_Invoice!$B$61</definedName>
+    <definedName name="Инвойс_получатель_п">Noncom_Invoice!$B$60</definedName>
     <definedName name="Инвойс_продавец">Noncom_Invoice!$B$4</definedName>
     <definedName name="Инвойс_продавец_адрес">Noncom_Invoice!$B$5</definedName>
-    <definedName name="Инвойс_продавец_адрес_п">Noncom_Invoice!$B$55</definedName>
-    <definedName name="Инвойс_продавец_п">Noncom_Invoice!$B$54</definedName>
+    <definedName name="Инвойс_продавец_адрес_п">Noncom_Invoice!$B$58</definedName>
+    <definedName name="Инвойс_продавец_п">Noncom_Invoice!$B$57</definedName>
     <definedName name="Инвойс_соглашение">Noncom_Invoice!$E$10</definedName>
-    <definedName name="Инвойс_соглашение_п">Noncom_Invoice!$E$60</definedName>
+    <definedName name="Инвойс_соглашение_п">Noncom_Invoice!$E$63</definedName>
     <definedName name="Инвойс_судно">Noncom_Invoice!$B$28</definedName>
-    <definedName name="Инвойс_судно_п">Noncom_Invoice!$B$77</definedName>
+    <definedName name="Инвойс_судно_п">Noncom_Invoice!$B$80</definedName>
     <definedName name="Инвойс_транспорт">Noncom_Invoice!$B$10</definedName>
-    <definedName name="Инвойс_транспорт_п">Noncom_Invoice!$B$60</definedName>
+    <definedName name="Инвойс_транспорт_п">Noncom_Invoice!$B$63</definedName>
     <definedName name="Контракт">Export_Storage_Contract!$B$2</definedName>
     <definedName name="Контракт_дата">Export_Storage_Contract!$B$3</definedName>
     <definedName name="Контракт_стороны">Export_Storage_Contract!$B$5</definedName>
     <definedName name="МСЦ">Noncom_Invoice!$G$4</definedName>
-    <definedName name="МСЦ_п">Noncom_Invoice!$G$54</definedName>
+    <definedName name="МСЦ_п">Noncom_Invoice!$G$57</definedName>
     <definedName name="МСЦ_сертификат">Noncom_Invoice!$H$4</definedName>
-    <definedName name="МСЦ_сертификат_п">Noncom_Invoice!$H$54</definedName>
+    <definedName name="МСЦ_сертификат_п">Noncom_Invoice!$H$57</definedName>
     <definedName name="Обязательство_хранение">Export_Storage_Contract!$B$6</definedName>
     <definedName name="Остальное_контракт">Export_Storage_Contract!$B$10</definedName>
     <definedName name="Сертификаты_массив">Export_Storage_Contract!$B$8</definedName>
@@ -1061,6 +1061,60 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1068,60 +1122,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1593,7 +1593,7 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
@@ -1727,14 +1727,14 @@
     </row>
     <row r="5" spans="1:24" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="87"/>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="122"/>
-      <c r="D5" s="108" t="s">
+      <c r="C5" s="108"/>
+      <c r="D5" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="109"/>
+      <c r="E5" s="106"/>
       <c r="F5" s="2"/>
       <c r="G5"/>
       <c r="H5"/>
@@ -1757,14 +1757,14 @@
     </row>
     <row r="6" spans="1:24" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="87"/>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="108" t="s">
+      <c r="C6" s="106"/>
+      <c r="D6" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="109"/>
+      <c r="E6" s="106"/>
       <c r="F6" s="2"/>
       <c r="G6"/>
       <c r="H6"/>
@@ -1855,14 +1855,14 @@
     </row>
     <row r="9" spans="1:24" s="100" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="89"/>
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="123" t="s">
+      <c r="C9" s="111"/>
+      <c r="D9" s="110" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="124"/>
+      <c r="E9" s="111"/>
       <c r="F9" s="91"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -1884,14 +1884,14 @@
     </row>
     <row r="10" spans="1:24" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="87"/>
-      <c r="B10" s="110" t="s">
+      <c r="B10" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="109"/>
-      <c r="D10" s="108" t="s">
+      <c r="C10" s="106"/>
+      <c r="D10" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="E10" s="109"/>
+      <c r="E10" s="106"/>
       <c r="F10" s="2"/>
       <c r="H10"/>
       <c r="I10"/>
@@ -1913,14 +1913,14 @@
     </row>
     <row r="11" spans="1:24" ht="55.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="87"/>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="109"/>
-      <c r="D11" s="108" t="s">
+      <c r="C11" s="106"/>
+      <c r="D11" s="105" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="109"/>
+      <c r="E11" s="106"/>
       <c r="F11" s="2"/>
       <c r="H11"/>
       <c r="I11"/>
@@ -1942,14 +1942,14 @@
     </row>
     <row r="12" spans="1:24" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="87"/>
-      <c r="B12" s="110" t="s">
+      <c r="B12" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="109"/>
-      <c r="D12" s="108" t="s">
+      <c r="C12" s="106"/>
+      <c r="D12" s="105" t="s">
         <v>102</v>
       </c>
-      <c r="E12" s="109"/>
+      <c r="E12" s="106"/>
       <c r="F12" s="2"/>
       <c r="H12"/>
       <c r="I12"/>
@@ -1971,14 +1971,14 @@
     </row>
     <row r="13" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="87"/>
-      <c r="B13" s="117" t="s">
+      <c r="B13" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="118"/>
-      <c r="D13" s="117" t="s">
+      <c r="C13" s="114"/>
+      <c r="D13" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="118"/>
+      <c r="E13" s="114"/>
       <c r="F13" s="2"/>
       <c r="H13"/>
       <c r="I13"/>
@@ -2000,218 +2000,218 @@
     </row>
     <row r="14" spans="1:24" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="87"/>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="120"/>
-      <c r="D14" s="119" t="s">
+      <c r="C14" s="116"/>
+      <c r="D14" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="120"/>
+      <c r="E14" s="116"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="87"/>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="114" t="s">
+      <c r="C15" s="118"/>
+      <c r="D15" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="115"/>
+      <c r="E15" s="118"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="87"/>
-      <c r="B16" s="110" t="s">
+      <c r="B16" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="108" t="s">
+      <c r="C16" s="106"/>
+      <c r="D16" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="109"/>
+      <c r="E16" s="106"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="87"/>
-      <c r="B17" s="110" t="s">
+      <c r="B17" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="109"/>
-      <c r="D17" s="108" t="s">
+      <c r="C17" s="106"/>
+      <c r="D17" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="109"/>
+      <c r="E17" s="106"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="87"/>
-      <c r="B18" s="110" t="s">
+      <c r="B18" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="109"/>
-      <c r="D18" s="108" t="s">
+      <c r="C18" s="106"/>
+      <c r="D18" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="109"/>
+      <c r="E18" s="106"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="87"/>
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="109"/>
-      <c r="D19" s="108" t="s">
+      <c r="C19" s="106"/>
+      <c r="D19" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="109"/>
+      <c r="E19" s="106"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="87"/>
-      <c r="B20" s="110" t="s">
+      <c r="B20" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="109"/>
-      <c r="D20" s="108" t="s">
+      <c r="C20" s="106"/>
+      <c r="D20" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="109"/>
+      <c r="E20" s="106"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="87"/>
-      <c r="B21" s="110" t="s">
+      <c r="B21" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="109"/>
-      <c r="D21" s="108" t="s">
+      <c r="C21" s="106"/>
+      <c r="D21" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="109"/>
+      <c r="E21" s="106"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="87"/>
-      <c r="B22" s="116" t="s">
+      <c r="B22" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="115"/>
-      <c r="D22" s="114" t="s">
+      <c r="C22" s="118"/>
+      <c r="D22" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="115"/>
+      <c r="E22" s="118"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="87"/>
-      <c r="B23" s="116" t="s">
+      <c r="B23" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="115"/>
-      <c r="D23" s="114" t="s">
+      <c r="C23" s="118"/>
+      <c r="D23" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="115"/>
+      <c r="E23" s="118"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="87"/>
-      <c r="B24" s="110" t="s">
+      <c r="B24" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="108" t="s">
+      <c r="C24" s="106"/>
+      <c r="D24" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="109"/>
+      <c r="E24" s="106"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="87"/>
-      <c r="B25" s="110" t="s">
+      <c r="B25" s="109" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="109"/>
-      <c r="D25" s="108" t="s">
+      <c r="C25" s="106"/>
+      <c r="D25" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="109"/>
+      <c r="E25" s="106"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="87"/>
-      <c r="B26" s="113" t="s">
+      <c r="B26" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="112"/>
-      <c r="D26" s="111" t="s">
+      <c r="C26" s="121"/>
+      <c r="D26" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="112"/>
+      <c r="E26" s="121"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="87"/>
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="112"/>
-      <c r="D27" s="111" t="s">
+      <c r="C27" s="121"/>
+      <c r="D27" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="112"/>
+      <c r="E27" s="121"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="87"/>
-      <c r="B28" s="110" t="s">
+      <c r="B28" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="109"/>
-      <c r="D28" s="108" t="s">
+      <c r="C28" s="106"/>
+      <c r="D28" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="109"/>
+      <c r="E28" s="106"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="87"/>
-      <c r="B29" s="110" t="s">
+      <c r="B29" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="109"/>
-      <c r="D29" s="108" t="s">
+      <c r="C29" s="106"/>
+      <c r="D29" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="109"/>
+      <c r="E29" s="106"/>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="87"/>
-      <c r="B30" s="110" t="s">
+      <c r="B30" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="109"/>
-      <c r="D30" s="108" t="s">
+      <c r="C30" s="106"/>
+      <c r="D30" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="109"/>
+      <c r="E30" s="106"/>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="42.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="87"/>
-      <c r="B31" s="107" t="s">
+      <c r="B31" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="106"/>
-      <c r="D31" s="105" t="s">
+      <c r="C31" s="124"/>
+      <c r="D31" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="106"/>
+      <c r="E31" s="124"/>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -2232,48 +2232,6 @@
     <row r="40" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B27:C27"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D28:E28"/>
@@ -2282,6 +2240,48 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:C7">
     <cfRule type="notContainsBlanks" dxfId="9" priority="21">
@@ -2346,10 +2346,10 @@
     <tabColor theme="8" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A31" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2358,7 +2358,7 @@
     <col min="2" max="2" width="15.265625" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.53125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13.3984375" customWidth="1"/>
     <col min="7" max="7" width="15.19921875" customWidth="1"/>
     <col min="8" max="8" width="15.53125" customWidth="1"/>
@@ -2975,259 +2975,253 @@
       <c r="G51" s="31"/>
       <c r="H51" s="31"/>
     </row>
-    <row r="52" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="B52" s="68" t="s">
+    <row r="52" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="40"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+    </row>
+    <row r="53" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="40"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+    </row>
+    <row r="54" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="40"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+    </row>
+    <row r="55" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="B55" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="68"/>
-      <c r="D52" s="68"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="3"/>
-      <c r="B53" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="F53" s="55"/>
-      <c r="G53" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="H53" s="104" t="s">
-        <v>41</v>
-      </c>
-      <c r="I53" s="84"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="3"/>
-      <c r="B54" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="F54" s="22"/>
-      <c r="G54" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H54" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="I54" s="84"/>
-    </row>
-    <row r="55" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="3"/>
-      <c r="B55" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="84"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="68"/>
     </row>
     <row r="56" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="3"/>
       <c r="B56" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="19"/>
-      <c r="E56" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="19"/>
+      <c r="E56" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="F56" s="55"/>
+      <c r="G56" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="H56" s="104" t="s">
+        <v>41</v>
+      </c>
       <c r="I56" s="84"/>
     </row>
     <row r="57" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="3"/>
       <c r="B57" s="21" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="22"/>
-      <c r="E57" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="22"/>
+      <c r="E57" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H57" s="38" t="s">
+        <v>74</v>
+      </c>
       <c r="I57" s="84"/>
     </row>
-    <row r="58" spans="1:9" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="3"/>
-      <c r="B58" s="133" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="133"/>
-      <c r="D58" s="134"/>
-      <c r="E58" s="135" t="s">
-        <v>120</v>
-      </c>
-      <c r="F58" s="128"/>
-      <c r="G58" s="128"/>
-      <c r="H58" s="129"/>
+      <c r="B58" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="24"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="27"/>
       <c r="I58" s="84"/>
     </row>
     <row r="59" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="3"/>
-      <c r="B59" s="80" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="57"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
-      <c r="H59" s="29"/>
+      <c r="B59" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="17"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="19"/>
       <c r="I59" s="84"/>
     </row>
     <row r="60" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="3"/>
-      <c r="B60" s="83" t="s">
+      <c r="B60" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="84"/>
+    </row>
+    <row r="61" spans="1:9" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="3"/>
+      <c r="B61" s="133" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="133"/>
+      <c r="D61" s="134"/>
+      <c r="E61" s="135" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" s="128"/>
+      <c r="G61" s="128"/>
+      <c r="H61" s="129"/>
+      <c r="I61" s="84"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="3"/>
+      <c r="B62" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="57"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="84"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="3"/>
+      <c r="B63" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="C60" s="30"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="60" t="s">
+      <c r="C63" s="30"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="F60" s="61"/>
-      <c r="G60" s="61"/>
-      <c r="H60" s="62"/>
-      <c r="I60" s="84"/>
-    </row>
-    <row r="61" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="3"/>
-      <c r="B61" s="33" t="s">
+      <c r="F63" s="61"/>
+      <c r="G63" s="61"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="84"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="3"/>
+      <c r="B64" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="33" t="s">
+      <c r="C64" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D61" s="34"/>
-      <c r="E61" s="20" t="s">
+      <c r="D64" s="34"/>
+      <c r="E64" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="84"/>
-    </row>
-    <row r="62" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="3"/>
-      <c r="B62" s="47" t="s">
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="84"/>
+    </row>
+    <row r="65" spans="1:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="3"/>
+      <c r="B65" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="C65" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D62" s="25"/>
-      <c r="E62" s="23" t="s">
+      <c r="D65" s="25"/>
+      <c r="E65" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="64"/>
-      <c r="I62" s="84"/>
-    </row>
-    <row r="63" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="3"/>
-      <c r="B63" s="65" t="s">
+      <c r="F65" s="63"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="64"/>
+      <c r="I65" s="84"/>
+    </row>
+    <row r="66" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="3"/>
+      <c r="B66" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C66" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D63" s="65" t="s">
+      <c r="D66" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="36" t="s">
+      <c r="E66" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="F63" s="36"/>
-      <c r="G63" s="65" t="s">
+      <c r="F66" s="36"/>
+      <c r="G66" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="H63" s="66" t="s">
+      <c r="H66" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="I63" s="84"/>
-    </row>
-    <row r="64" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="3"/>
-      <c r="B64" s="69" t="s">
+      <c r="I66" s="84"/>
+    </row>
+    <row r="67" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="3"/>
+      <c r="B67" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C64" s="69" t="s">
+      <c r="C67" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="D64" s="69" t="s">
+      <c r="D67" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="E64" s="69">
+      <c r="E67" s="69">
         <v>426</v>
       </c>
-      <c r="F64" s="69" t="s">
+      <c r="F67" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="G64" s="69" t="s">
+      <c r="G67" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="H64" s="75" t="s">
+      <c r="H67" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="I64" s="84"/>
-    </row>
-    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="3"/>
-      <c r="B65" s="40"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="84"/>
-    </row>
-    <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="3"/>
-      <c r="B66" s="40"/>
-      <c r="C66" s="41"/>
-      <c r="D66" s="53"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="84"/>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="3"/>
-      <c r="B67" s="40"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="72"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="40"/>
-      <c r="H67" s="38"/>
       <c r="I67" s="84"/>
     </row>
-    <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="3"/>
       <c r="B68" s="40"/>
       <c r="C68" s="41"/>
@@ -3260,7 +3254,7 @@
       <c r="H70" s="38"/>
       <c r="I70" s="84"/>
     </row>
-    <row r="71" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="3"/>
       <c r="B71" s="40"/>
       <c r="C71" s="41"/>
@@ -3282,7 +3276,7 @@
       <c r="H72" s="38"/>
       <c r="I72" s="84"/>
     </row>
-    <row r="73" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="3"/>
       <c r="B73" s="40"/>
       <c r="C73" s="41"/>
@@ -3293,7 +3287,7 @@
       <c r="H73" s="38"/>
       <c r="I73" s="84"/>
     </row>
-    <row r="74" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="3"/>
       <c r="B74" s="40"/>
       <c r="C74" s="41"/>
@@ -3304,114 +3298,144 @@
       <c r="H74" s="38"/>
       <c r="I74" s="84"/>
     </row>
-    <row r="75" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="3"/>
-      <c r="B75" s="76"/>
-      <c r="C75" s="76"/>
-      <c r="D75" s="76"/>
-      <c r="E75" s="76"/>
-      <c r="F75" s="76"/>
-      <c r="G75" s="76"/>
-      <c r="H75" s="14"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="72"/>
+      <c r="F75" s="40"/>
+      <c r="G75" s="40"/>
+      <c r="H75" s="38"/>
       <c r="I75" s="84"/>
     </row>
-    <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="3"/>
-      <c r="B76" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="C76" s="77"/>
-      <c r="D76" s="77"/>
-      <c r="E76" s="77"/>
-      <c r="F76" s="77"/>
-      <c r="G76" s="77"/>
-      <c r="H76" s="67"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="41"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="72"/>
+      <c r="F76" s="40"/>
+      <c r="G76" s="40"/>
+      <c r="H76" s="38"/>
       <c r="I76" s="84"/>
     </row>
-    <row r="77" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="3"/>
-      <c r="B77" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="11"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="41"/>
+      <c r="D77" s="53"/>
+      <c r="E77" s="72"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="40"/>
+      <c r="H77" s="38"/>
       <c r="I77" s="84"/>
     </row>
-    <row r="78" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="3"/>
-      <c r="B78" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="11"/>
+      <c r="B78" s="76"/>
+      <c r="C78" s="76"/>
+      <c r="D78" s="76"/>
+      <c r="E78" s="76"/>
+      <c r="F78" s="76"/>
+      <c r="G78" s="76"/>
+      <c r="H78" s="14"/>
       <c r="I78" s="84"/>
     </row>
     <row r="79" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="3"/>
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="C79" s="77"/>
+      <c r="D79" s="77"/>
+      <c r="E79" s="77"/>
+      <c r="F79" s="77"/>
+      <c r="G79" s="77"/>
+      <c r="H79" s="67"/>
+      <c r="I79" s="84"/>
+    </row>
+    <row r="80" spans="1:9" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="3"/>
+      <c r="B80" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="84"/>
+    </row>
+    <row r="81" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="3"/>
+      <c r="B81" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="84"/>
+    </row>
+    <row r="82" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="3"/>
+      <c r="B82" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="84"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A80" s="3"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="41"/>
-      <c r="D80" s="43" t="s">
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="84"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A83" s="3"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="41"/>
+      <c r="D83" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E80" s="42" t="s">
+      <c r="E83" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="F80" s="43" t="s">
+      <c r="F83" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="H80" s="42" t="s">
+      <c r="H83" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="I80" s="84"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A81" s="3"/>
-      <c r="B81" s="40"/>
-      <c r="C81" s="41"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="45"/>
-      <c r="F81" s="46"/>
-      <c r="G81" s="45"/>
-      <c r="H81" s="48"/>
-      <c r="I81" s="84"/>
-    </row>
-    <row r="82" spans="1:9" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="3"/>
-      <c r="B82" s="82"/>
-      <c r="C82" s="49"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="51" t="s">
+      <c r="I83" s="84"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A84" s="3"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="41"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="45"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="45"/>
+      <c r="H84" s="48"/>
+      <c r="I84" s="84"/>
+    </row>
+    <row r="85" spans="1:9" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="3"/>
+      <c r="B85" s="82"/>
+      <c r="C85" s="49"/>
+      <c r="D85" s="50"/>
+      <c r="E85" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="F82" s="51"/>
-      <c r="G82" s="51"/>
-      <c r="H82" s="52"/>
-      <c r="I82" s="84"/>
-    </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
+      <c r="F85" s="51"/>
+      <c r="G85" s="51"/>
+      <c r="H85" s="52"/>
+      <c r="I85" s="84"/>
+    </row>
     <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
@@ -3419,16 +3443,19 @@
     <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:H8"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="E58:H58"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="E61:H61"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="90" fitToHeight="2" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="88" fitToHeight="2" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
beta r contract with auto images added, need to fix storage contract tmp init
</commit_message>
<xml_diff>
--- a/templates/Export_Storage_Agreement.xlsx
+++ b/templates/Export_Storage_Agreement.xlsx
@@ -8,30 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1233E5A-8226-4161-914B-E637A467F61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E06BB1C-6454-4091-BFE5-1C3B22BDDBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16996" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Storage_Contract" sheetId="1" r:id="rId1"/>
     <sheet name="Noncom_Invoice" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Storage_Contract!$A$1:$K$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Storage_Contract!$A$1:$K$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Noncom_Invoice!$A$1:$J$107</definedName>
+    <definedName name="Seal_agent_end">Export_Storage_Contract!$I$34</definedName>
+    <definedName name="Seal_agent_start">Export_Storage_Contract!$H$25</definedName>
+    <definedName name="Seal_seller_end">Export_Storage_Contract!$C$34</definedName>
+    <definedName name="Seal_seller_start">Export_Storage_Contract!$C$27</definedName>
+    <definedName name="Sign_agent_end">Export_Storage_Contract!$H$34</definedName>
+    <definedName name="Sign_agent_start">Export_Storage_Contract!$H$32</definedName>
+    <definedName name="Sign_seller_end">Export_Storage_Contract!$C$37</definedName>
+    <definedName name="Sign_seller_start">Export_Storage_Contract!$C$32</definedName>
     <definedName name="Адреса_банк_получателя">Export_Storage_Contract!$B$17</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Storage_Contract!$B$18</definedName>
     <definedName name="Адреса_банк_получателя_свифт">Export_Storage_Contract!$B$19</definedName>
     <definedName name="Адреса_заголовок">Export_Storage_Contract!$B$13</definedName>
-    <definedName name="Адреса_подпись">Export_Storage_Contract!$B$32</definedName>
+    <definedName name="Адреса_подпись">Export_Storage_Contract!$B$33</definedName>
     <definedName name="Адреса_покупатель">Export_Storage_Contract!$B$23</definedName>
     <definedName name="Адреса_покупатель_адрес">Export_Storage_Contract!$B$24</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Storage_Contract!$B$25</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Storage_Contract!$B$27</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Storage_Contract!$B$26</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Storage_Contract!$B$28</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Storage_Contract!$B$29</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Storage_Contract!$B$30</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Storage_Contract!$B$26</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Storage_Contract!$B$28</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Storage_Contract!$B$27</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Storage_Contract!$B$29</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Storage_Contract!$B$30</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Storage_Contract!$B$31</definedName>
     <definedName name="Адреса_получатель_в_пользу">Export_Storage_Contract!$B$20</definedName>
     <definedName name="Адреса_получатель_счет">Export_Storage_Contract!$B$21</definedName>
     <definedName name="Адреса_продавец">Export_Storage_Contract!$B$15</definedName>
@@ -110,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="136">
   <si>
     <t>KTI COMPANY LIMITED ( Korea, Busan) ,  here in after referred to as Contractor, represented by the President SE JI YOUNG on one part, and "Tikhrybcom Co., LTD", (Russia, Magadan), here in after referred to asCustomer, represented by the  Deputy General Director M.N. Kruzina, acting on the basis of the Charter, on the other part, have concluded this Supplementary Agreement on the following:</t>
   </si>
@@ -525,6 +533,9 @@
   </si>
   <si>
     <t>4. Настоящее дополнительное соглашение вступает в силу с момента его подписания и является неотъемлемой частью контракта оказания услуг хранения №344/33957322/0157 от  02.04.2018</t>
+  </si>
+  <si>
+    <t>Shinpyung branch</t>
   </si>
 </sst>
 </file>
@@ -785,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1061,9 +1072,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1089,6 +1097,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1116,15 +1184,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1134,27 +1193,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1164,66 +1211,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1253,6 +1246,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1684,24 +1689,24 @@
     <tabColor theme="8" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC42"/>
+  <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:J24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.53125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.53125" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.265625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.19921875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.19921875" style="1" customWidth="1"/>
     <col min="11" max="11" width="1.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.796875" style="1"/>
     <col min="13" max="13" width="16.796875" style="1" customWidth="1"/>
@@ -1722,19 +1727,19 @@
   <sheetData>
     <row r="1" spans="1:29" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="80"/>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="130" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="111" t="s">
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="130" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="113"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="132"/>
       <c r="K1" s="2"/>
       <c r="M1"/>
       <c r="N1"/>
@@ -1754,19 +1759,19 @@
     </row>
     <row r="2" spans="1:29" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="80"/>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="114" t="s">
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="116"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="135"/>
       <c r="K2" s="2"/>
       <c r="M2"/>
       <c r="N2"/>
@@ -1786,19 +1791,19 @@
     </row>
     <row r="3" spans="1:29" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="81"/>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="136" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="117" t="s">
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="136" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="119"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="138"/>
       <c r="K3" s="83"/>
       <c r="M3" s="90"/>
       <c r="N3" s="90"/>
@@ -1844,21 +1849,21 @@
       <c r="Z4" s="90"/>
       <c r="AA4" s="90"/>
     </row>
-    <row r="5" spans="1:29" ht="95.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29" ht="82.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="80"/>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="135"/>
-      <c r="G5" s="120" t="s">
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="121"/>
-      <c r="I5" s="121"/>
-      <c r="J5" s="122"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="117"/>
       <c r="K5" s="2"/>
       <c r="L5"/>
       <c r="M5"/>
@@ -1881,19 +1886,19 @@
     </row>
     <row r="6" spans="1:29" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="80"/>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="123" t="s">
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="139" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="125"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="141"/>
       <c r="K6" s="2"/>
       <c r="L6"/>
       <c r="M6"/>
@@ -1909,29 +1914,27 @@
       <c r="W6"/>
       <c r="X6"/>
       <c r="Y6"/>
-      <c r="Z6" s="85" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z6"/>
       <c r="AA6"/>
       <c r="AB6"/>
       <c r="AC6"/>
     </row>
     <row r="7" spans="1:29" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="80"/>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="144"/>
+      <c r="D7" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="130" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
-      <c r="G7" s="151" t="s">
+      <c r="E7" s="143"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="152"/>
-      <c r="I7" s="152"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
       <c r="J7" s="85" t="s">
         <v>125</v>
       </c>
@@ -1950,34 +1953,38 @@
       <c r="W7"/>
       <c r="X7"/>
       <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
+      <c r="Z7" s="160" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="160"/>
+      <c r="AB7" s="161"/>
       <c r="AC7"/>
     </row>
     <row r="8" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="80"/>
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="127" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="128"/>
+      <c r="D8" s="127" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="127"/>
-      <c r="D8" s="132" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="132"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="126" t="s">
+      <c r="E8" s="129"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="127" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="132"/>
-      <c r="I8" s="132"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="128"/>
       <c r="J8" s="92" t="s">
         <v>121</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
+      <c r="M8" s="127" t="s">
+        <v>119</v>
+      </c>
+      <c r="N8" s="128"/>
       <c r="O8"/>
       <c r="P8"/>
       <c r="Q8"/>
@@ -1989,28 +1996,26 @@
       <c r="W8"/>
       <c r="X8"/>
       <c r="Y8"/>
-      <c r="Z8" s="92" t="s">
-        <v>118</v>
-      </c>
+      <c r="Z8"/>
       <c r="AA8"/>
       <c r="AB8"/>
       <c r="AC8"/>
     </row>
     <row r="9" spans="1:29" s="91" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="82"/>
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
-      <c r="F9" s="141"/>
-      <c r="G9" s="153" t="s">
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="112"/>
+      <c r="G9" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="155"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="112"/>
       <c r="K9" s="84"/>
       <c r="M9"/>
       <c r="N9"/>
@@ -2032,19 +2037,19 @@
     </row>
     <row r="10" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="80"/>
-      <c r="B10" s="120" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="133" t="s">
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H10" s="134"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="135"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="2"/>
       <c r="M10"/>
       <c r="N10"/>
@@ -2066,19 +2071,19 @@
     </row>
     <row r="11" spans="1:29" ht="55.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="80"/>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="133" t="s">
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="135"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="2"/>
       <c r="M11"/>
       <c r="N11"/>
@@ -2100,19 +2105,19 @@
     </row>
     <row r="12" spans="1:29" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="80"/>
-      <c r="B12" s="120" t="s">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="133" t="s">
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="134"/>
-      <c r="I12" s="134"/>
-      <c r="J12" s="135"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="2"/>
       <c r="M12"/>
       <c r="N12"/>
@@ -2134,19 +2139,19 @@
     </row>
     <row r="13" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="80"/>
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="137"/>
-      <c r="D13" s="137"/>
-      <c r="E13" s="137"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="136" t="s">
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="137"/>
-      <c r="I13" s="137"/>
-      <c r="J13" s="138"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="123"/>
       <c r="K13" s="2"/>
       <c r="M13"/>
       <c r="N13"/>
@@ -2168,463 +2173,452 @@
     </row>
     <row r="14" spans="1:29" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="80"/>
-      <c r="B14" s="145" t="s">
+      <c r="B14" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="146"/>
-      <c r="D14" s="146"/>
-      <c r="E14" s="146"/>
-      <c r="F14" s="147"/>
-      <c r="G14" s="145" t="s">
+      <c r="C14" s="125"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="125"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="146"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="147"/>
+      <c r="H14" s="125"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="126"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="80"/>
-      <c r="B15" s="142" t="s">
+      <c r="B15" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="143"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="143"/>
-      <c r="F15" s="144"/>
-      <c r="G15" s="142" t="s">
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="143"/>
-      <c r="I15" s="143"/>
-      <c r="J15" s="144"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="120"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="80"/>
-      <c r="B16" s="120" t="s">
+      <c r="B16" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
-      <c r="E16" s="121"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="120" t="s">
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="121"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="122"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="117"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="80"/>
-      <c r="B17" s="120" t="s">
+      <c r="B17" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="120" t="s">
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="122"/>
+      <c r="H17" s="116"/>
+      <c r="I17" s="116"/>
+      <c r="J17" s="117"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="80"/>
-      <c r="B18" s="120" t="s">
+      <c r="B18" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="121"/>
-      <c r="D18" s="121"/>
-      <c r="E18" s="121"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="120" t="s">
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="121"/>
-      <c r="I18" s="121"/>
-      <c r="J18" s="122"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="117"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="80"/>
-      <c r="B19" s="120" t="s">
+      <c r="B19" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="122"/>
-      <c r="G19" s="120" t="s">
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="121"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="122"/>
+      <c r="H19" s="116"/>
+      <c r="I19" s="116"/>
+      <c r="J19" s="117"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="80"/>
-      <c r="B20" s="120" t="s">
+      <c r="B20" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
-      <c r="F20" s="122"/>
-      <c r="G20" s="120" t="s">
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="121"/>
-      <c r="I20" s="121"/>
-      <c r="J20" s="122"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="117"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="80"/>
-      <c r="B21" s="120" t="s">
+      <c r="B21" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="121"/>
-      <c r="D21" s="121"/>
-      <c r="E21" s="121"/>
-      <c r="F21" s="122"/>
-      <c r="G21" s="120" t="s">
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="121"/>
-      <c r="I21" s="121"/>
-      <c r="J21" s="122"/>
+      <c r="H21" s="116"/>
+      <c r="I21" s="116"/>
+      <c r="J21" s="117"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="80"/>
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="143"/>
-      <c r="D22" s="143"/>
-      <c r="E22" s="143"/>
-      <c r="F22" s="144"/>
-      <c r="G22" s="142" t="s">
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="143"/>
-      <c r="I22" s="143"/>
-      <c r="J22" s="144"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="120"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="80"/>
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="143"/>
-      <c r="D23" s="143"/>
-      <c r="E23" s="143"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="142" t="s">
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="143"/>
-      <c r="I23" s="143"/>
-      <c r="J23" s="144"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="120"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="80"/>
-      <c r="B24" s="120" t="s">
+      <c r="B24" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="121"/>
-      <c r="D24" s="121"/>
-      <c r="E24" s="121"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="120" t="s">
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="121"/>
-      <c r="I24" s="121"/>
-      <c r="J24" s="122"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="116"/>
+      <c r="J24" s="117"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="1.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="80"/>
-      <c r="B25" s="120" t="s">
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="114"/>
+      <c r="H25" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="103"/>
+      <c r="J25" s="114"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="80"/>
+      <c r="B26" s="113" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="120" t="s">
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="114"/>
+      <c r="G26" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="121"/>
-      <c r="I25" s="121"/>
-      <c r="J25" s="122"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="80"/>
-      <c r="B26" s="148" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="149"/>
-      <c r="D26" s="149"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="150"/>
-      <c r="G26" s="148" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="149"/>
-      <c r="I26" s="149"/>
-      <c r="J26" s="150"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="114"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="80"/>
-      <c r="B27" s="101" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="103"/>
-      <c r="D27" s="103"/>
-      <c r="E27" s="103"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="106" t="s">
-        <v>133</v>
-      </c>
-      <c r="H27" s="107" t="s">
+      <c r="B27" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="I27" s="107"/>
-      <c r="J27" s="108"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="105" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="107"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="80"/>
-      <c r="B28" s="101" t="s">
+      <c r="B28" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="104" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="104"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="106" t="s">
+      <c r="D28" s="102"/>
+      <c r="E28" s="102"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="H28" s="104"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="5"/>
+      <c r="I28" s="106"/>
+      <c r="J28" s="107"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="80"/>
-      <c r="B29" s="101" t="s">
+      <c r="B29" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="104"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="103"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="106" t="s">
+      <c r="G29" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="96"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="5"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="80"/>
-      <c r="B30" s="101" t="s">
+      <c r="B30" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="104"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="103"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="106" t="s">
+      <c r="G30" s="105" t="s">
         <v>133</v>
       </c>
       <c r="H30" s="104"/>
       <c r="I30" s="104"/>
-      <c r="J30" s="5"/>
+      <c r="J30" s="96"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="80"/>
-      <c r="B31" s="104"/>
-      <c r="C31" s="104"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="104"/>
+      <c r="B31" s="105" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="103"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="104"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
+      <c r="G31" s="105" t="s">
+        <v>133</v>
+      </c>
+      <c r="H31" s="103"/>
+      <c r="I31" s="103"/>
       <c r="J31" s="5"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="41.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="80"/>
-      <c r="B32" s="102" t="s">
-        <v>31</v>
-      </c>
+      <c r="B32" s="103"/>
       <c r="C32" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="102"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="99"/>
-      <c r="G32" s="98" t="s">
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="101" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" s="79"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="80"/>
+      <c r="B33" s="101" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="101"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="102" t="s">
+      <c r="I33" s="101"/>
+      <c r="J33" s="97"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="80"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="I32" s="102"/>
-      <c r="J32" s="97"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="80"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="109" t="s">
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="86"/>
-      <c r="H33" s="109" t="s">
+      <c r="I34" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="I33" s="88"/>
-      <c r="J33" s="87"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="110" t="s">
-        <v>116</v>
-      </c>
-      <c r="I34" s="110" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G36" s="98"/>
-    </row>
-    <row r="37" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:11" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="109"/>
+      <c r="G37" s="98"/>
+    </row>
     <row r="38" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B8:C8"/>
+  <mergeCells count="41">
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G6:J6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
   </mergeCells>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="6">
+      <formula>LEN(TRIM(D7))&gt;0</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="7">
+      <formula>LEN(TRIM(D7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8 G8 J8">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="10">
+      <formula>LEN(TRIM(B8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z7 G7:J7">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="22">
+      <formula>LEN(TRIM(G7))&gt;0</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="23">
+      <formula>LEN(TRIM(G7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(D8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8 G8:J8">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(B8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7 G7:J7">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="19">
-      <formula>LEN(TRIM(D7))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
-      <formula>LEN(TRIM(D7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
-      <formula>LEN(TRIM(D8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z6">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="5">
-      <formula>LEN(TRIM(Z6))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="1" priority="6">
-      <formula>LEN(TRIM(Z6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z8">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(Z8))&gt;0</formula>
+  <conditionalFormatting sqref="M8">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(M8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="92" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -2725,12 +2719,12 @@
     </row>
     <row r="6" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="157"/>
+      <c r="C6" s="150"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="151"/>
       <c r="F6" s="12" t="s">
         <v>39</v>
       </c>
@@ -2757,18 +2751,18 @@
     </row>
     <row r="8" spans="1:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
-      <c r="B8" s="158" t="s">
+      <c r="B8" s="152" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="158"/>
-      <c r="D8" s="158"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="160" t="s">
+      <c r="C8" s="152"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="154" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="161"/>
-      <c r="H8" s="161"/>
-      <c r="I8" s="162"/>
+      <c r="G8" s="155"/>
+      <c r="H8" s="155"/>
+      <c r="I8" s="156"/>
       <c r="J8" s="78"/>
     </row>
     <row r="9" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3528,18 +3522,18 @@
     </row>
     <row r="68" spans="1:10" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="3"/>
-      <c r="B68" s="163" t="s">
+      <c r="B68" s="157" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="163"/>
-      <c r="D68" s="163"/>
-      <c r="E68" s="164"/>
-      <c r="F68" s="165" t="s">
+      <c r="C68" s="157"/>
+      <c r="D68" s="157"/>
+      <c r="E68" s="158"/>
+      <c r="F68" s="159" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="158"/>
-      <c r="H68" s="158"/>
-      <c r="I68" s="159"/>
+      <c r="G68" s="152"/>
+      <c r="H68" s="152"/>
+      <c r="I68" s="153"/>
       <c r="J68" s="78"/>
     </row>
     <row r="69" spans="1:10" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
r contract implemented, some logic generalized in high order functions in createExportContract, need to add picture feature in exportDefaultContract tmp
</commit_message>
<xml_diff>
--- a/templates/Export_Storage_Agreement.xlsx
+++ b/templates/Export_Storage_Agreement.xlsx
@@ -8,43 +8,43 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E06BB1C-6454-4091-BFE5-1C3B22BDDBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A53D09-F0D0-4FCF-BF8E-52A165823597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Export_Storage_Contract" sheetId="1" r:id="rId1"/>
+    <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
     <sheet name="Noncom_Invoice" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Storage_Contract!$A$1:$K$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$I$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Noncom_Invoice!$A$1:$J$107</definedName>
-    <definedName name="Seal_agent_end">Export_Storage_Contract!$I$34</definedName>
-    <definedName name="Seal_agent_start">Export_Storage_Contract!$H$25</definedName>
-    <definedName name="Seal_seller_end">Export_Storage_Contract!$C$34</definedName>
-    <definedName name="Seal_seller_start">Export_Storage_Contract!$C$27</definedName>
-    <definedName name="Sign_agent_end">Export_Storage_Contract!$H$34</definedName>
-    <definedName name="Sign_agent_start">Export_Storage_Contract!$H$32</definedName>
-    <definedName name="Sign_seller_end">Export_Storage_Contract!$C$37</definedName>
-    <definedName name="Sign_seller_start">Export_Storage_Contract!$C$32</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Storage_Contract!$B$17</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Storage_Contract!$B$18</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Storage_Contract!$B$19</definedName>
-    <definedName name="Адреса_заголовок">Export_Storage_Contract!$B$13</definedName>
-    <definedName name="Адреса_подпись">Export_Storage_Contract!$B$33</definedName>
-    <definedName name="Адреса_покупатель">Export_Storage_Contract!$B$23</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Storage_Contract!$B$24</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Storage_Contract!$B$26</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Storage_Contract!$B$28</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Storage_Contract!$B$27</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Storage_Contract!$B$29</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Storage_Contract!$B$30</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Storage_Contract!$B$31</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Storage_Contract!$B$20</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Storage_Contract!$B$21</definedName>
-    <definedName name="Адреса_продавец">Export_Storage_Contract!$B$15</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Storage_Contract!$B$16</definedName>
-    <definedName name="Доставка_транспорт">Export_Storage_Contract!$B$9</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$G$34</definedName>
+    <definedName name="Seal_agent_start">Export_Contract!$F$25</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$34</definedName>
+    <definedName name="Seal_seller_start">Export_Contract!$C$27</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$F$34</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$F$32</definedName>
+    <definedName name="Sign_seller_end">Export_Contract!$C$37</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$32</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$B$17</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$18</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$19</definedName>
+    <definedName name="Адреса_заголовок">Export_Contract!$B$13</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$33</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$B$23</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$24</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$26</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$28</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$27</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$29</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$30</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$31</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$20</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$B$21</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$B$15</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$16</definedName>
+    <definedName name="Доставка_транспорт">Export_Contract!$B$9</definedName>
     <definedName name="Инвойс">Noncom_Invoice!$F$4</definedName>
     <definedName name="Инвойс_Bl_массив">Noncom_Invoice!$B$14</definedName>
     <definedName name="Инвойс_Bl_массив_п">Noncom_Invoice!$B$74</definedName>
@@ -83,19 +83,19 @@
     <definedName name="Инвойс_судно_п">Noncom_Invoice!#REF!</definedName>
     <definedName name="Инвойс_транспорт">Noncom_Invoice!$B$10</definedName>
     <definedName name="Инвойс_транспорт_п">Noncom_Invoice!$B$70</definedName>
-    <definedName name="Контракт">Export_Storage_Contract!$B$2</definedName>
-    <definedName name="Контракт_дата">Export_Storage_Contract!$B$3</definedName>
-    <definedName name="Контракт_стороны">Export_Storage_Contract!$B$5</definedName>
+    <definedName name="Контракт">Export_Contract!$B$2</definedName>
+    <definedName name="Контракт_дата">Export_Contract!$B$3</definedName>
+    <definedName name="Контракт_стороны">Export_Contract!$B$5</definedName>
     <definedName name="МСЦ">Noncom_Invoice!$H$4</definedName>
     <definedName name="МСЦ_п">Noncom_Invoice!$H$64</definedName>
     <definedName name="МСЦ_сертификат">Noncom_Invoice!$I$4</definedName>
     <definedName name="МСЦ_сертификат_п">Noncom_Invoice!$I$64</definedName>
-    <definedName name="Обязательство_хранение">Export_Storage_Contract!$B$6</definedName>
-    <definedName name="Остальное_контракт">Export_Storage_Contract!$B$10</definedName>
-    <definedName name="Сертификаты_массив">Export_Storage_Contract!$B$8</definedName>
-    <definedName name="Соглашение">Export_Storage_Contract!$B$1</definedName>
-    <definedName name="Соглашение_вступление">Export_Storage_Contract!$B$11</definedName>
-    <definedName name="Юридикция">Export_Storage_Contract!$B$12</definedName>
+    <definedName name="Обязательство_хранение">Export_Contract!$B$6</definedName>
+    <definedName name="Остальное_контракт">Export_Contract!$B$10</definedName>
+    <definedName name="Сертификаты_массив">Export_Contract!$B$8</definedName>
+    <definedName name="Соглашение">Export_Contract!$B$1</definedName>
+    <definedName name="Соглашение_вступление">Export_Contract!$B$11</definedName>
+    <definedName name="Юридикция">Export_Contract!$B$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="136">
   <si>
     <t>KTI COMPANY LIMITED ( Korea, Busan) ,  here in after referred to as Contractor, represented by the President SE JI YOUNG on one part, and "Tikhrybcom Co., LTD", (Russia, Magadan), here in after referred to asCustomer, represented by the  Deputy General Director M.N. Kruzina, acting on the basis of the Charter, on the other part, have concluded this Supplementary Agreement on the following:</t>
   </si>
@@ -796,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1066,12 +1066,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1112,41 +1106,98 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1157,60 +1208,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1246,31 +1243,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -1305,36 +1283,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1689,10 +1637,10 @@
     <tabColor theme="8" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC43"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
@@ -1700,47 +1648,45 @@
     <col min="1" max="1" width="1.796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.53125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.265625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.19921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="1.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.796875" style="1"/>
-    <col min="13" max="13" width="16.796875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="20.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="15.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="49.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="13.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="7.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="9.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.796875" style="1"/>
+    <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.53125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.19921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="1.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.796875" style="1"/>
+    <col min="11" max="11" width="16.796875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.796875" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="49.796875" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="13.796875" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="7.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.796875" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="80"/>
-      <c r="B1" s="130" t="s">
+      <c r="B1" s="128" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="130" t="s">
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="2"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="2"/>
+      <c r="K1"/>
+      <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
       <c r="O1"/>
@@ -1754,25 +1700,23 @@
       <c r="W1"/>
       <c r="X1"/>
       <c r="Y1"/>
-      <c r="Z1"/>
-      <c r="AA1"/>
-    </row>
-    <row r="2" spans="1:29" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:27" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="80"/>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="130" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="133" t="s">
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="130" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="2"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="2"/>
+      <c r="K2"/>
+      <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
@@ -1786,25 +1730,23 @@
       <c r="W2"/>
       <c r="X2"/>
       <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-    </row>
-    <row r="3" spans="1:29" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:27" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="81"/>
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="132" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="136" t="s">
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="132" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="83"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="83"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
       <c r="M3" s="90"/>
       <c r="N3" s="90"/>
       <c r="O3" s="90"/>
@@ -1818,21 +1760,19 @@
       <c r="W3" s="90"/>
       <c r="X3" s="90"/>
       <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="90"/>
-    </row>
-    <row r="4" spans="1:29" s="89" customFormat="1" ht="6.4" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:27" s="89" customFormat="1" ht="6.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="81"/>
       <c r="B4" s="79"/>
       <c r="C4" s="79"/>
       <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="79"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="83"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="83"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
       <c r="M4" s="90"/>
       <c r="N4" s="90"/>
       <c r="O4" s="90"/>
@@ -1846,25 +1786,23 @@
       <c r="W4" s="90"/>
       <c r="X4" s="90"/>
       <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-    </row>
-    <row r="5" spans="1:29" ht="82.9" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:27" ht="82.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="80"/>
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="146"/>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="147"/>
-      <c r="G5" s="115" t="s">
+      <c r="C5" s="135"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="116" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="2"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="2"/>
+      <c r="J5"/>
+      <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
@@ -1881,25 +1819,23 @@
       <c r="Y5"/>
       <c r="Z5"/>
       <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-    </row>
-    <row r="6" spans="1:29" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:27" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="80"/>
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="141"/>
-      <c r="G6" s="139" t="s">
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="136" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="141"/>
-      <c r="K6" s="2"/>
+      <c r="F6" s="137"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="141"/>
+      <c r="I6" s="2"/>
+      <c r="J6"/>
+      <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6"/>
@@ -1916,29 +1852,27 @@
       <c r="Y6"/>
       <c r="Z6"/>
       <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-    </row>
-    <row r="7" spans="1:29" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="80"/>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="144"/>
-      <c r="D7" s="142" t="s">
+      <c r="C7" s="143"/>
+      <c r="D7" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="143"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="148" t="s">
+      <c r="E7" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="149"/>
-      <c r="I7" s="149"/>
-      <c r="J7" s="85" t="s">
+      <c r="F7" s="148"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7"/>
+      <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -1953,38 +1887,32 @@
       <c r="W7"/>
       <c r="X7"/>
       <c r="Y7"/>
-      <c r="Z7" s="160" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA7" s="160"/>
-      <c r="AB7" s="161"/>
-      <c r="AC7"/>
-    </row>
-    <row r="8" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Z7"/>
+      <c r="AA7"/>
+    </row>
+    <row r="8" spans="1:27" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="80"/>
-      <c r="B8" s="127" t="s">
+      <c r="B8" s="144" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="128"/>
-      <c r="D8" s="127" t="s">
+      <c r="C8" s="145"/>
+      <c r="D8" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="129"/>
-      <c r="F8" s="128"/>
-      <c r="G8" s="127" t="s">
+      <c r="E8" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="129"/>
-      <c r="I8" s="128"/>
-      <c r="J8" s="92" t="s">
+      <c r="F8" s="146"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8"/>
+      <c r="K8"/>
       <c r="L8"/>
-      <c r="M8" s="127" t="s">
-        <v>119</v>
-      </c>
-      <c r="N8" s="128"/>
+      <c r="M8"/>
+      <c r="N8"/>
       <c r="O8"/>
       <c r="P8"/>
       <c r="Q8"/>
@@ -1998,25 +1926,23 @@
       <c r="Y8"/>
       <c r="Z8"/>
       <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-    </row>
-    <row r="9" spans="1:29" s="91" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:27" s="91" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="82"/>
-      <c r="B9" s="110" t="s">
+      <c r="B9" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="110" t="s">
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="84"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="84"/>
+      <c r="K9"/>
+      <c r="L9"/>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
@@ -2032,25 +1958,23 @@
       <c r="Y9"/>
       <c r="Z9"/>
       <c r="AA9"/>
-      <c r="AB9"/>
-      <c r="AC9"/>
-    </row>
-    <row r="10" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:27" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="80"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="79"/>
       <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="2"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="2"/>
+      <c r="K10"/>
+      <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10"/>
@@ -2066,25 +1990,23 @@
       <c r="Y10"/>
       <c r="Z10"/>
       <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-    </row>
-    <row r="11" spans="1:29" ht="55.15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:27" ht="55.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="80"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="79"/>
       <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="2"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="2"/>
+      <c r="K11"/>
+      <c r="L11"/>
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
@@ -2100,25 +2022,23 @@
       <c r="Y11"/>
       <c r="Z11"/>
       <c r="AA11"/>
-      <c r="AB11"/>
-      <c r="AC11"/>
-    </row>
-    <row r="12" spans="1:29" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:27" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="80"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="79"/>
       <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="2"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="2"/>
+      <c r="K12"/>
+      <c r="L12"/>
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
@@ -2134,25 +2054,23 @@
       <c r="Y12"/>
       <c r="Z12"/>
       <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-    </row>
-    <row r="13" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="80"/>
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="122"/>
-      <c r="D13" s="122"/>
-      <c r="E13" s="122"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="121" t="s">
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="120" t="s">
         <v>9</v>
       </c>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
       <c r="H13" s="122"/>
-      <c r="I13" s="122"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="K13"/>
+      <c r="L13"/>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
@@ -2168,457 +2086,397 @@
       <c r="Y13"/>
       <c r="Z13"/>
       <c r="AA13"/>
-      <c r="AB13"/>
-      <c r="AC13"/>
-    </row>
-    <row r="14" spans="1:29" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:27" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="80"/>
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="124" t="s">
+      <c r="C14" s="124"/>
+      <c r="D14" s="124"/>
+      <c r="E14" s="123" t="s">
         <v>11</v>
       </c>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
       <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="126"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="80"/>
       <c r="B15" s="118" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="119"/>
       <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="118" t="s">
+      <c r="E15" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="119"/>
-      <c r="I15" s="119"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="126"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="80"/>
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="116" t="s">
+        <v>15</v>
+      </c>
       <c r="F16" s="117"/>
-      <c r="G16" s="115" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="117"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="117"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="80"/>
-      <c r="B17" s="115" t="s">
+      <c r="B17" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="116" t="s">
+        <v>17</v>
+      </c>
       <c r="F17" s="117"/>
-      <c r="G17" s="115" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="117"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="117"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="80"/>
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="116" t="s">
+        <v>19</v>
+      </c>
       <c r="F18" s="117"/>
-      <c r="G18" s="115" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="117"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="80"/>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="116" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="117"/>
-      <c r="G19" s="115" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="116"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="117"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="117"/>
+      <c r="H19" s="127"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="80"/>
-      <c r="B20" s="115" t="s">
+      <c r="B20" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="116" t="s">
+        <v>21</v>
+      </c>
       <c r="F20" s="117"/>
-      <c r="G20" s="115" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="116"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="117"/>
+      <c r="H20" s="127"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="80"/>
-      <c r="B21" s="115" t="s">
+      <c r="B21" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="116"/>
-      <c r="D21" s="116"/>
-      <c r="E21" s="116"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="116" t="s">
+        <v>23</v>
+      </c>
       <c r="F21" s="117"/>
-      <c r="G21" s="115" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="116"/>
-      <c r="I21" s="116"/>
-      <c r="J21" s="117"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="117"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="80"/>
       <c r="B22" s="118" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="119"/>
       <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="118" t="s">
+      <c r="E22" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="119"/>
-      <c r="I22" s="119"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="119"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="126"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="80"/>
       <c r="B23" s="118" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="119"/>
       <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="120"/>
-      <c r="G23" s="118" t="s">
+      <c r="E23" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="119"/>
-      <c r="I23" s="119"/>
-      <c r="J23" s="120"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F23" s="119"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="126"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="80"/>
-      <c r="B24" s="115" t="s">
+      <c r="B24" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="116"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="116"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="116" t="s">
+        <v>28</v>
+      </c>
       <c r="F24" s="117"/>
-      <c r="G24" s="115" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="116"/>
-      <c r="I24" s="116"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" ht="1.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="117"/>
+      <c r="H24" s="127"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="80"/>
-      <c r="C25" s="103"/>
-      <c r="D25" s="103"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="114"/>
-      <c r="H25" s="106" t="s">
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
+      <c r="F25" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="I25" s="103"/>
-      <c r="J25" s="114"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="101"/>
+      <c r="H25" s="112"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="80"/>
-      <c r="B26" s="113" t="s">
+      <c r="B26" s="111" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="113" t="s">
+      <c r="C26" s="101"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="103"/>
-      <c r="J26" s="114"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="101"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="80"/>
-      <c r="B27" s="105" t="s">
+      <c r="B27" s="103" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="105" t="s">
+      <c r="D27" s="104"/>
+      <c r="E27" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="104"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="80"/>
-      <c r="B28" s="105" t="s">
+      <c r="B28" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="102"/>
-      <c r="E28" s="102"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="105" t="s">
+      <c r="D28" s="100"/>
+      <c r="E28" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="I28" s="106"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="104"/>
+      <c r="H28" s="105"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="80"/>
-      <c r="B29" s="105" t="s">
+      <c r="B29" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="103"/>
-      <c r="E29" s="103"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="105" t="s">
+      <c r="D29" s="101"/>
+      <c r="E29" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="H29" s="103"/>
-      <c r="I29" s="103"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="101"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="80"/>
-      <c r="B30" s="105" t="s">
+      <c r="B30" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="D30" s="103"/>
-      <c r="E30" s="103"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="105" t="s">
+      <c r="D30" s="101"/>
+      <c r="E30" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="H30" s="104"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="96"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F30" s="102"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="96"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="80"/>
-      <c r="B31" s="105" t="s">
+      <c r="B31" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="105" t="s">
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="80"/>
-      <c r="B32" s="103"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="103"/>
-      <c r="H32" s="101" t="s">
+      <c r="D32" s="101"/>
+      <c r="E32" s="111"/>
+      <c r="F32" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="I32" s="79"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G32" s="79"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="80"/>
-      <c r="B33" s="101" t="s">
+      <c r="B33" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="101"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="98" t="s">
+      <c r="D33" s="99"/>
+      <c r="E33" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="101"/>
-      <c r="J33" s="97"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="99"/>
+      <c r="H33" s="97"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="80"/>
       <c r="B34" s="88"/>
-      <c r="C34" s="108" t="s">
+      <c r="C34" s="106" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="108" t="s">
+      <c r="E34" s="86"/>
+      <c r="F34" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="I34" s="108" t="s">
+      <c r="G34" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="J34" s="87"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:11" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="109"/>
-      <c r="G37" s="98"/>
-    </row>
-    <row r="38" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" ht="10.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:9" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="107"/>
+      <c r="E37" s="98"/>
+    </row>
+    <row r="38" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="38">
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="M8:N8"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="6">
-      <formula>LEN(TRIM(D7))&gt;0</formula>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
+      <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="7">
-      <formula>LEN(TRIM(D7))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="3">
+      <formula>LEN(TRIM(B7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8 G8 J8">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="10">
+  <conditionalFormatting sqref="B8 H8">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="10">
       <formula>LEN(TRIM(B8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z7 G7:J7">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="22">
-      <formula>LEN(TRIM(G7))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="23">
-      <formula>LEN(TRIM(G7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+  <conditionalFormatting sqref="D8:E8">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(D8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="2">
-      <formula>LEN(TRIM(B7))&gt;0</formula>
+  <conditionalFormatting sqref="D7:H7">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="6">
+      <formula>LEN(TRIM(D7))&gt;0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(B7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(M8))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
+      <formula>LEN(TRIM(D7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="91" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="92" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -2719,12 +2577,12 @@
     </row>
     <row r="6" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="150" t="s">
+      <c r="B6" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="151"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="150"/>
       <c r="F6" s="12" t="s">
         <v>39</v>
       </c>
@@ -2751,18 +2609,18 @@
     </row>
     <row r="8" spans="1:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="151" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="152"/>
-      <c r="D8" s="152"/>
-      <c r="E8" s="153"/>
-      <c r="F8" s="154" t="s">
+      <c r="C8" s="151"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="153" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="155"/>
-      <c r="H8" s="155"/>
-      <c r="I8" s="156"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
+      <c r="I8" s="155"/>
       <c r="J8" s="78"/>
     </row>
     <row r="9" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3522,18 +3380,18 @@
     </row>
     <row r="68" spans="1:10" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="3"/>
-      <c r="B68" s="157" t="s">
+      <c r="B68" s="156" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="157"/>
-      <c r="D68" s="157"/>
-      <c r="E68" s="158"/>
-      <c r="F68" s="159" t="s">
+      <c r="C68" s="156"/>
+      <c r="D68" s="156"/>
+      <c r="E68" s="157"/>
+      <c r="F68" s="158" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="152"/>
-      <c r="H68" s="152"/>
-      <c r="I68" s="153"/>
+      <c r="G68" s="151"/>
+      <c r="H68" s="151"/>
+      <c r="I68" s="152"/>
       <c r="J68" s="78"/>
     </row>
     <row r="69" spans="1:10" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
insert rows bugs fixed + old tmp returned back
</commit_message>
<xml_diff>
--- a/templates/Export_Storage_Agreement.xlsx
+++ b/templates/Export_Storage_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BA5DEA-282C-41AA-B4A0-6C7E332788F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BF8611-40DD-49B8-9348-475DC3CE6365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16996" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -1237,6 +1237,126 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1244,126 +1364,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1791,8 +1791,8 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
@@ -1825,17 +1825,17 @@
   <sheetData>
     <row r="1" spans="1:29" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="80"/>
-      <c r="B1" s="139" t="s">
+      <c r="B1" s="142" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="139" t="s">
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="141"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="144"/>
       <c r="I1" s="2"/>
       <c r="K1"/>
       <c r="L1"/>
@@ -1855,17 +1855,17 @@
     </row>
     <row r="2" spans="1:29" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="80"/>
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="145" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="142" t="s">
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="145" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="144"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="147"/>
       <c r="I2" s="2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -1885,17 +1885,17 @@
     </row>
     <row r="3" spans="1:29" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="81"/>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="148" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="145" t="s">
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="147"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="150"/>
       <c r="I3" s="83"/>
       <c r="K3" s="90"/>
       <c r="L3" s="90"/>
@@ -1914,17 +1914,17 @@
       <c r="Y3" s="90"/>
     </row>
     <row r="4" spans="1:29" s="116" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="154" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="152"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="151" t="s">
+      <c r="C4" s="155"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="154" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="153"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="156"/>
       <c r="I4" s="117"/>
       <c r="M4" s="91"/>
       <c r="Z4" s="91"/>
@@ -1933,17 +1933,17 @@
       <c r="AC4" s="91"/>
     </row>
     <row r="5" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="157" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="129" t="s">
+      <c r="C5" s="158"/>
+      <c r="D5" s="159"/>
+      <c r="E5" s="157" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="131"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="158"/>
+      <c r="H5" s="159"/>
       <c r="I5" s="118"/>
       <c r="K5" s="119"/>
       <c r="M5" s="1"/>
@@ -1953,17 +1953,17 @@
       <c r="AC5" s="1"/>
     </row>
     <row r="6" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="160" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="126" t="s">
+      <c r="C6" s="161"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="128"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="161"/>
+      <c r="H6" s="162"/>
       <c r="I6" s="120"/>
       <c r="M6" s="1"/>
       <c r="Z6" s="1"/>
@@ -1972,17 +1972,17 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="163" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="123" t="s">
+      <c r="C7" s="164"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="125"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="165"/>
       <c r="I7" s="121"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -2003,17 +2003,17 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="163" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="124"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="123" t="s">
+      <c r="C8" s="164"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="163" t="s">
         <v>141</v>
       </c>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="125"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="165"/>
       <c r="I8" s="121"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -2034,17 +2034,17 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="163" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="123" t="s">
+      <c r="C9" s="164"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="163" t="s">
         <v>143</v>
       </c>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="125"/>
+      <c r="F9" s="164"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="165"/>
       <c r="I9" s="121"/>
       <c r="M9" s="91"/>
       <c r="Z9" s="91"/>
@@ -2053,17 +2053,17 @@
       <c r="AC9" s="91"/>
     </row>
     <row r="10" spans="1:29" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="129" t="s">
+      <c r="B10" s="157" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="130"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="129" t="s">
+      <c r="C10" s="158"/>
+      <c r="D10" s="159"/>
+      <c r="E10" s="157" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="130"/>
-      <c r="G10" s="130"/>
-      <c r="H10" s="131"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="158"/>
+      <c r="H10" s="159"/>
       <c r="I10" s="118"/>
       <c r="M10" s="1"/>
       <c r="Z10" s="1"/>
@@ -2072,68 +2072,68 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:29" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="126" t="s">
+      <c r="B11" s="160" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="126" t="s">
+      <c r="C11" s="161"/>
+      <c r="D11" s="162"/>
+      <c r="E11" s="160" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="127"/>
-      <c r="G11" s="127"/>
-      <c r="H11" s="128"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="162"/>
       <c r="I11" s="120"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" customFormat="1" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="124"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="123" t="s">
+      <c r="C12" s="164"/>
+      <c r="D12" s="165"/>
+      <c r="E12" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="125"/>
+      <c r="F12" s="164"/>
+      <c r="G12" s="164"/>
+      <c r="H12" s="165"/>
       <c r="I12" s="121"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" customFormat="1" ht="11.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="163" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="124"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="123" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="163" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
-      <c r="H13" s="125"/>
+      <c r="F13" s="164"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="165"/>
       <c r="I13" s="121"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="1:29" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="123" t="s">
+      <c r="B14" s="163" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="124"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="123" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="163" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="124"/>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
+      <c r="F14" s="164"/>
+      <c r="G14" s="164"/>
+      <c r="H14" s="164"/>
       <c r="I14" s="122"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -2141,17 +2141,17 @@
     </row>
     <row r="15" spans="1:29" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="80"/>
-      <c r="B15" s="148" t="s">
+      <c r="B15" s="151" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="149"/>
-      <c r="D15" s="149"/>
-      <c r="E15" s="148" t="s">
+      <c r="C15" s="152"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="149"/>
-      <c r="G15" s="149"/>
-      <c r="H15" s="150"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="153"/>
       <c r="I15" s="2"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -2174,18 +2174,18 @@
     </row>
     <row r="16" spans="1:29" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="80"/>
-      <c r="B16" s="132" t="s">
+      <c r="B16" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="133"/>
+      <c r="C16" s="136"/>
       <c r="D16" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="137" t="s">
+      <c r="E16" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="138"/>
-      <c r="G16" s="138"/>
+      <c r="F16" s="141"/>
+      <c r="G16" s="141"/>
       <c r="H16" s="85" t="s">
         <v>123</v>
       </c>
@@ -2211,18 +2211,18 @@
     </row>
     <row r="17" spans="1:27" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="80"/>
-      <c r="B17" s="134" t="s">
+      <c r="B17" s="137" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="135"/>
+      <c r="C17" s="138"/>
       <c r="D17" s="113" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="134" t="s">
+      <c r="E17" s="137" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="136"/>
-      <c r="G17" s="135"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="138"/>
       <c r="H17" s="92" t="s">
         <v>119</v>
       </c>
@@ -2376,17 +2376,17 @@
     </row>
     <row r="22" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="80"/>
-      <c r="B22" s="156" t="s">
+      <c r="B22" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="157"/>
-      <c r="D22" s="157"/>
-      <c r="E22" s="156" t="s">
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="157"/>
-      <c r="G22" s="157"/>
-      <c r="H22" s="162"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="129"/>
       <c r="I22" s="2"/>
       <c r="K22"/>
       <c r="L22"/>
@@ -2408,167 +2408,167 @@
     </row>
     <row r="23" spans="1:27" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="80"/>
-      <c r="B23" s="160" t="s">
+      <c r="B23" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="161"/>
-      <c r="D23" s="161"/>
-      <c r="E23" s="160" t="s">
+      <c r="C23" s="131"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="161"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="163"/>
+      <c r="F23" s="131"/>
+      <c r="G23" s="131"/>
+      <c r="H23" s="132"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="80"/>
-      <c r="B24" s="158" t="s">
+      <c r="B24" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="159"/>
-      <c r="D24" s="159"/>
-      <c r="E24" s="158" t="s">
+      <c r="C24" s="126"/>
+      <c r="D24" s="126"/>
+      <c r="E24" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="159"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="164"/>
+      <c r="F24" s="126"/>
+      <c r="G24" s="126"/>
+      <c r="H24" s="133"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="80"/>
-      <c r="B25" s="154" t="s">
+      <c r="B25" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="155"/>
-      <c r="D25" s="155"/>
-      <c r="E25" s="154" t="s">
+      <c r="C25" s="124"/>
+      <c r="D25" s="124"/>
+      <c r="E25" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="155"/>
-      <c r="G25" s="155"/>
-      <c r="H25" s="165"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="134"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="80"/>
-      <c r="B26" s="154" t="s">
+      <c r="B26" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="155"/>
-      <c r="D26" s="155"/>
-      <c r="E26" s="154" t="s">
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="155"/>
-      <c r="G26" s="155"/>
-      <c r="H26" s="165"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="134"/>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="80"/>
-      <c r="B27" s="154" t="s">
+      <c r="B27" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="155"/>
-      <c r="D27" s="155"/>
-      <c r="E27" s="154" t="s">
+      <c r="C27" s="124"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="155"/>
-      <c r="G27" s="155"/>
-      <c r="H27" s="165"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="134"/>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="80"/>
-      <c r="B28" s="154" t="s">
+      <c r="B28" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="155"/>
-      <c r="D28" s="155"/>
-      <c r="E28" s="154" t="s">
+      <c r="C28" s="124"/>
+      <c r="D28" s="124"/>
+      <c r="E28" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="155"/>
-      <c r="G28" s="155"/>
-      <c r="H28" s="165"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="134"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="80"/>
-      <c r="B29" s="154" t="s">
+      <c r="B29" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="155"/>
-      <c r="D29" s="155"/>
-      <c r="E29" s="154" t="s">
+      <c r="C29" s="124"/>
+      <c r="D29" s="124"/>
+      <c r="E29" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="155"/>
-      <c r="G29" s="155"/>
-      <c r="H29" s="165"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="124"/>
+      <c r="H29" s="134"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="80"/>
-      <c r="B30" s="154" t="s">
+      <c r="B30" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="154" t="s">
+      <c r="C30" s="124"/>
+      <c r="D30" s="124"/>
+      <c r="E30" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
-      <c r="H30" s="165"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="124"/>
+      <c r="H30" s="134"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="80"/>
-      <c r="B31" s="158" t="s">
+      <c r="B31" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="159"/>
-      <c r="D31" s="159"/>
-      <c r="E31" s="158" t="s">
+      <c r="C31" s="126"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="159"/>
-      <c r="G31" s="159"/>
-      <c r="H31" s="164"/>
+      <c r="F31" s="126"/>
+      <c r="G31" s="126"/>
+      <c r="H31" s="133"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="80"/>
-      <c r="B32" s="158" t="s">
+      <c r="B32" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="159"/>
-      <c r="D32" s="159"/>
-      <c r="E32" s="158" t="s">
+      <c r="C32" s="126"/>
+      <c r="D32" s="126"/>
+      <c r="E32" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="159"/>
-      <c r="G32" s="159"/>
-      <c r="H32" s="164"/>
+      <c r="F32" s="126"/>
+      <c r="G32" s="126"/>
+      <c r="H32" s="133"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="80"/>
-      <c r="B33" s="154" t="s">
+      <c r="B33" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="155"/>
-      <c r="D33" s="155"/>
-      <c r="E33" s="154" t="s">
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="155"/>
-      <c r="G33" s="155"/>
-      <c r="H33" s="165"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="124"/>
+      <c r="H33" s="134"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2728,6 +2728,48 @@
     <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B31:D31"/>
@@ -2744,48 +2786,6 @@
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="E31:H31"/>
     <mergeCell ref="E32:H32"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="B16">
     <cfRule type="notContainsBlanks" dxfId="5" priority="2">

</xml_diff>

<commit_message>
sale invoice group rows feature checkbox added
</commit_message>
<xml_diff>
--- a/templates/Export_Storage_Agreement.xlsx
+++ b/templates/Export_Storage_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01199DA0-00B9-4592-8A07-40BABDE73033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB48CA51-3E88-4A80-B989-83CF01EB9018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23760" yWindow="3247" windowWidth="21600" windowHeight="11423" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{F7A04C55-AC1F-405E-AB59-9B2973B4CD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="MID_Contract">Export_Contract!$D$1</definedName>
-    <definedName name="MID_Invoice">Invoice!$F$1</definedName>
+    <definedName name="MID_Invoice">Invoice!$G$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$2:$I$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$2:$N$48</definedName>
     <definedName name="Seal_agent_end">Export_Contract!$G$44</definedName>
@@ -819,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1101,9 +1101,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1168,21 +1165,132 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1204,131 +1312,65 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1725,8 +1767,8 @@
   </sheetPr>
   <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
@@ -1764,17 +1806,17 @@
     </row>
     <row r="2" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="23"/>
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="179" t="s">
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="181"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="150"/>
       <c r="I2" s="2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -1794,17 +1836,17 @@
     </row>
     <row r="3" spans="1:29" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23"/>
-      <c r="B3" s="158" t="s">
+      <c r="B3" s="151" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="158" t="s">
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="160"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="153"/>
       <c r="I3" s="2"/>
       <c r="K3"/>
       <c r="L3"/>
@@ -1824,17 +1866,17 @@
     </row>
     <row r="4" spans="1:29" s="32" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="24"/>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="161" t="s">
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="162"/>
-      <c r="G4" s="162"/>
-      <c r="H4" s="163"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="156"/>
       <c r="I4" s="26"/>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
@@ -1853,17 +1895,17 @@
       <c r="Y4" s="33"/>
     </row>
     <row r="5" spans="1:29" s="56" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="167" t="s">
+      <c r="B5" s="160" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="168"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="167" t="s">
+      <c r="C5" s="161"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="160" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="168"/>
-      <c r="G5" s="168"/>
-      <c r="H5" s="169"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="162"/>
       <c r="I5" s="57"/>
       <c r="M5" s="34"/>
       <c r="Z5" s="34"/>
@@ -1872,17 +1914,17 @@
       <c r="AC5" s="34"/>
     </row>
     <row r="6" spans="1:29" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="170" t="s">
+      <c r="B6" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="170" t="s">
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="171"/>
-      <c r="G6" s="171"/>
-      <c r="H6" s="172"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="138"/>
       <c r="I6" s="62"/>
       <c r="K6" s="63"/>
       <c r="M6" s="1"/>
@@ -1892,17 +1934,17 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="163" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="149"/>
-      <c r="D7" s="150"/>
-      <c r="E7" s="148" t="s">
+      <c r="C7" s="164"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="163" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="149"/>
-      <c r="G7" s="149"/>
-      <c r="H7" s="150"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="165"/>
       <c r="I7" s="59"/>
       <c r="M7" s="1"/>
       <c r="Z7" s="1"/>
@@ -1911,17 +1953,17 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="166" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="143"/>
-      <c r="D8" s="144"/>
-      <c r="E8" s="142" t="s">
+      <c r="C8" s="167"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="144"/>
+      <c r="F8" s="167"/>
+      <c r="G8" s="167"/>
+      <c r="H8" s="168"/>
       <c r="I8" s="60"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1942,17 +1984,17 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="142" t="s">
+      <c r="B9" s="166" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="143"/>
-      <c r="D9" s="144"/>
-      <c r="E9" s="142" t="s">
+      <c r="C9" s="167"/>
+      <c r="D9" s="168"/>
+      <c r="E9" s="166" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="143"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="144"/>
+      <c r="F9" s="167"/>
+      <c r="G9" s="167"/>
+      <c r="H9" s="168"/>
       <c r="I9" s="60"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1973,17 +2015,17 @@
       <c r="AC9" s="1"/>
     </row>
     <row r="10" spans="1:29" customFormat="1" ht="11.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="143"/>
-      <c r="D10" s="144"/>
-      <c r="E10" s="142" t="s">
+      <c r="C10" s="167"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="143"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="144"/>
+      <c r="F10" s="167"/>
+      <c r="G10" s="167"/>
+      <c r="H10" s="168"/>
       <c r="I10" s="60"/>
       <c r="M10" s="34"/>
       <c r="Z10" s="34"/>
@@ -1992,17 +2034,17 @@
       <c r="AC10" s="34"/>
     </row>
     <row r="11" spans="1:29" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="145" t="s">
+      <c r="B11" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="146"/>
-      <c r="D11" s="146"/>
-      <c r="E11" s="145" t="s">
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="147"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="132"/>
+      <c r="H11" s="139"/>
       <c r="I11" s="58"/>
       <c r="M11" s="1"/>
       <c r="Z11" s="1"/>
@@ -2011,68 +2053,68 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="148" t="s">
+      <c r="B12" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="149"/>
-      <c r="D12" s="150"/>
-      <c r="E12" s="148" t="s">
+      <c r="C12" s="164"/>
+      <c r="D12" s="165"/>
+      <c r="E12" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="149"/>
-      <c r="G12" s="149"/>
-      <c r="H12" s="150"/>
+      <c r="F12" s="164"/>
+      <c r="G12" s="164"/>
+      <c r="H12" s="165"/>
       <c r="I12" s="59"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" customFormat="1" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="142" t="s">
+      <c r="B13" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="143"/>
-      <c r="D13" s="144"/>
-      <c r="E13" s="142" t="s">
+      <c r="C13" s="167"/>
+      <c r="D13" s="168"/>
+      <c r="E13" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="144"/>
+      <c r="F13" s="167"/>
+      <c r="G13" s="167"/>
+      <c r="H13" s="168"/>
       <c r="I13" s="60"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="1:29" customFormat="1" ht="11.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="166" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="143"/>
-      <c r="D14" s="144"/>
-      <c r="E14" s="142" t="s">
+      <c r="C14" s="167"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="166" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="143"/>
-      <c r="G14" s="143"/>
-      <c r="H14" s="144"/>
+      <c r="F14" s="167"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="168"/>
       <c r="I14" s="60"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
     </row>
     <row r="15" spans="1:29" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="142" t="s">
+      <c r="B15" s="166" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="143"/>
-      <c r="D15" s="144"/>
-      <c r="E15" s="142" t="s">
+      <c r="C15" s="167"/>
+      <c r="D15" s="168"/>
+      <c r="E15" s="166" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="143"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="143"/>
+      <c r="F15" s="167"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
       <c r="I15" s="61"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -2080,17 +2122,17 @@
     </row>
     <row r="16" spans="1:29" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="23"/>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="157" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="165"/>
-      <c r="E16" s="164" t="s">
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="165"/>
-      <c r="G16" s="165"/>
-      <c r="H16" s="166"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="159"/>
       <c r="I16" s="2"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -2113,18 +2155,18 @@
     </row>
     <row r="17" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="23"/>
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="152"/>
+      <c r="C17" s="142"/>
       <c r="D17" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="156" t="s">
+      <c r="E17" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="157"/>
-      <c r="G17" s="157"/>
+      <c r="F17" s="147"/>
+      <c r="G17" s="147"/>
       <c r="H17" s="28" t="s">
         <v>54</v>
       </c>
@@ -2150,18 +2192,18 @@
     </row>
     <row r="18" spans="1:27" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="23"/>
-      <c r="B18" s="153" t="s">
+      <c r="B18" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="154"/>
+      <c r="C18" s="144"/>
       <c r="D18" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="153" t="s">
+      <c r="E18" s="143" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="155"/>
-      <c r="G18" s="154"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="144"/>
       <c r="H18" s="35" t="s">
         <v>52</v>
       </c>
@@ -2315,17 +2357,17 @@
     </row>
     <row r="23" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="23"/>
-      <c r="B23" s="175" t="s">
+      <c r="B23" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="176"/>
-      <c r="D23" s="176"/>
-      <c r="E23" s="175" t="s">
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="176"/>
-      <c r="G23" s="176"/>
-      <c r="H23" s="177"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="136"/>
+      <c r="H23" s="137"/>
       <c r="I23" s="2"/>
       <c r="K23"/>
       <c r="L23"/>
@@ -2347,167 +2389,167 @@
     </row>
     <row r="24" spans="1:27" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="23"/>
-      <c r="B24" s="170" t="s">
+      <c r="B24" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="171"/>
-      <c r="D24" s="171"/>
-      <c r="E24" s="170" t="s">
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="171"/>
-      <c r="G24" s="171"/>
-      <c r="H24" s="172"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="138"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="23"/>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="146"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="145" t="s">
+      <c r="C25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="147"/>
+      <c r="F25" s="132"/>
+      <c r="G25" s="132"/>
+      <c r="H25" s="139"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="23"/>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="174"/>
-      <c r="D26" s="174"/>
-      <c r="E26" s="173" t="s">
+      <c r="C26" s="130"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="174"/>
-      <c r="G26" s="174"/>
-      <c r="H26" s="178"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="140"/>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
-      <c r="B27" s="173" t="s">
+      <c r="B27" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="174"/>
-      <c r="D27" s="174"/>
-      <c r="E27" s="173" t="s">
+      <c r="C27" s="130"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="174"/>
-      <c r="G27" s="174"/>
-      <c r="H27" s="178"/>
+      <c r="F27" s="130"/>
+      <c r="G27" s="130"/>
+      <c r="H27" s="140"/>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="23"/>
-      <c r="B28" s="173" t="s">
+      <c r="B28" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="174"/>
-      <c r="E28" s="173" t="s">
+      <c r="C28" s="130"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
-      <c r="H28" s="178"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="140"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="23"/>
-      <c r="B29" s="173" t="s">
+      <c r="B29" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="174"/>
-      <c r="D29" s="174"/>
-      <c r="E29" s="173" t="s">
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="174"/>
-      <c r="G29" s="174"/>
-      <c r="H29" s="178"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="140"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="23"/>
-      <c r="B30" s="173" t="s">
+      <c r="B30" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="174"/>
-      <c r="D30" s="174"/>
-      <c r="E30" s="173" t="s">
+      <c r="C30" s="130"/>
+      <c r="D30" s="130"/>
+      <c r="E30" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="174"/>
-      <c r="G30" s="174"/>
-      <c r="H30" s="178"/>
+      <c r="F30" s="130"/>
+      <c r="G30" s="130"/>
+      <c r="H30" s="140"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
-      <c r="B31" s="173" t="s">
+      <c r="B31" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="174"/>
-      <c r="D31" s="174"/>
-      <c r="E31" s="173" t="s">
+      <c r="C31" s="130"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="174"/>
-      <c r="G31" s="174"/>
-      <c r="H31" s="178"/>
+      <c r="F31" s="130"/>
+      <c r="G31" s="130"/>
+      <c r="H31" s="140"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23"/>
-      <c r="B32" s="170" t="s">
+      <c r="B32" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="171"/>
-      <c r="D32" s="171"/>
-      <c r="E32" s="170" t="s">
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="171"/>
-      <c r="G32" s="171"/>
-      <c r="H32" s="172"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="138"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23"/>
-      <c r="B33" s="145" t="s">
+      <c r="B33" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="146"/>
-      <c r="D33" s="146"/>
-      <c r="E33" s="145" t="s">
+      <c r="C33" s="132"/>
+      <c r="D33" s="132"/>
+      <c r="E33" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="146"/>
-      <c r="G33" s="146"/>
-      <c r="H33" s="147"/>
+      <c r="F33" s="132"/>
+      <c r="G33" s="132"/>
+      <c r="H33" s="139"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23"/>
-      <c r="B34" s="173" t="s">
+      <c r="B34" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="174"/>
-      <c r="D34" s="174"/>
-      <c r="E34" s="173" t="s">
+      <c r="C34" s="130"/>
+      <c r="D34" s="130"/>
+      <c r="E34" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
-      <c r="H34" s="178"/>
+      <c r="F34" s="130"/>
+      <c r="G34" s="130"/>
+      <c r="H34" s="140"/>
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2667,6 +2709,48 @@
     <row r="53" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B32:D32"/>
@@ -2683,48 +2767,6 @@
     <mergeCell ref="E30:H30"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="E33:H33"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B17">
     <cfRule type="notContainsBlanks" dxfId="5" priority="2">
@@ -2772,8 +2814,8 @@
   </sheetPr>
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2787,7 +2829,7 @@
     <col min="7" max="7" width="0.796875" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="10.73046875" customWidth="1"/>
-    <col min="10" max="10" width="13.265625" customWidth="1"/>
+    <col min="10" max="10" width="14.19921875" customWidth="1"/>
     <col min="11" max="11" width="8.06640625" customWidth="1"/>
     <col min="12" max="12" width="9.1328125" customWidth="1"/>
     <col min="13" max="13" width="15.53125" customWidth="1"/>
@@ -2797,89 +2839,89 @@
     <col min="22" max="22" width="13.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="3.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F1" s="132" t="s">
+    <row r="1" spans="1:20" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G1" s="128" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="36.85" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="93"/>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="111" t="s">
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="21"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="176"/>
     </row>
     <row r="3" spans="1:20" ht="32.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="93"/>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="113" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="114" t="s">
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="113" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="21"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="176"/>
     </row>
     <row r="4" spans="1:20" s="33" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="95"/>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="116" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="119" t="s">
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="118" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
-      <c r="L4" s="117"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
       <c r="M4" s="117"/>
       <c r="N4" s="94"/>
     </row>
     <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="93"/>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="121" t="s">
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
+      <c r="I5" s="179"/>
+      <c r="J5" s="179"/>
+      <c r="K5" s="179"/>
+      <c r="L5" s="179"/>
+      <c r="M5" s="180"/>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:20" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -2894,29 +2936,31 @@
       <c r="H6" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="182"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
       <c r="H7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="183"/>
+      <c r="K7" s="183"/>
+      <c r="L7" s="182"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="92" t="s">
@@ -2930,11 +2974,12 @@
       <c r="H8" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="131"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="85"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="184"/>
+      <c r="L8" s="182"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="91" t="s">
@@ -2948,47 +2993,50 @@
       <c r="H9" s="87" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
+      <c r="I9" s="182"/>
+      <c r="J9" s="182"/>
+      <c r="K9" s="182"/>
+      <c r="L9" s="182"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="21"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="127"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="127"/>
       <c r="H10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="85"/>
+      <c r="I10" s="182"/>
+      <c r="J10" s="182"/>
+      <c r="K10" s="182"/>
+      <c r="L10" s="182"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="21"/>
     </row>
     <row r="11" spans="1:20" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="136" t="s">
+      <c r="B11" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
+      <c r="C11" s="173"/>
+      <c r="D11" s="173"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="173"/>
       <c r="G11" s="100"/>
-      <c r="H11" s="136" t="s">
+      <c r="H11" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="137"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="137"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
+      <c r="I11" s="185"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="185"/>
+      <c r="M11" s="186"/>
+      <c r="N11" s="21"/>
     </row>
     <row r="12" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="91" t="s">
@@ -3002,54 +3050,57 @@
       <c r="H12" s="91" t="s">
         <v>104</v>
       </c>
-      <c r="I12" s="128"/>
-      <c r="J12" s="128"/>
-      <c r="K12" s="128"/>
-      <c r="L12" s="85"/>
-      <c r="M12" s="85"/>
+      <c r="I12" s="181"/>
+      <c r="J12" s="181"/>
+      <c r="K12" s="181"/>
+      <c r="L12" s="182"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="129"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
-      <c r="G13" s="129"/>
+      <c r="C13" s="127"/>
+      <c r="D13" s="127"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="127"/>
       <c r="H13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="130"/>
-      <c r="J13" s="130"/>
-      <c r="K13" s="130"/>
-      <c r="L13" s="85"/>
-      <c r="M13" s="85"/>
-    </row>
-    <row r="14" spans="1:20" ht="41.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="136" t="s">
+      <c r="I13" s="183"/>
+      <c r="J13" s="183"/>
+      <c r="K13" s="183"/>
+      <c r="L13" s="182"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="21"/>
+    </row>
+    <row r="14" spans="1:20" ht="48.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="194" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
-      <c r="F14" s="137"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="136" t="s">
+      <c r="C14" s="195"/>
+      <c r="D14" s="195"/>
+      <c r="E14" s="195"/>
+      <c r="F14" s="195"/>
+      <c r="G14" s="196"/>
+      <c r="H14" s="194" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="137"/>
-      <c r="J14" s="137"/>
-      <c r="K14" s="137"/>
-      <c r="L14" s="137"/>
-      <c r="M14" s="137"/>
+      <c r="I14" s="195"/>
+      <c r="J14" s="195"/>
+      <c r="K14" s="195"/>
+      <c r="L14" s="195"/>
+      <c r="M14" s="197"/>
+      <c r="N14" s="21"/>
     </row>
     <row r="15" spans="1:20" ht="30.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="90"/>
-      <c r="B15" s="125" t="s">
+      <c r="B15" s="124" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="126"/>
+      <c r="C15" s="125"/>
       <c r="D15" s="83" t="s">
         <v>91</v>
       </c>
@@ -3058,18 +3109,18 @@
         <v>94</v>
       </c>
       <c r="G15" s="83"/>
-      <c r="H15" s="125" t="s">
+      <c r="H15" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="I15" s="83"/>
-      <c r="J15" s="86" t="s">
+      <c r="I15" s="187"/>
+      <c r="J15" s="188" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86" t="s">
+      <c r="K15" s="188"/>
+      <c r="L15" s="188" t="s">
         <v>92</v>
       </c>
-      <c r="M15" s="127"/>
+      <c r="M15" s="126"/>
       <c r="N15" s="21"/>
       <c r="P15" s="83"/>
       <c r="S15" s="83"/>
@@ -3092,12 +3143,12 @@
       <c r="H16" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="105" t="s">
+      <c r="I16" s="189"/>
+      <c r="J16" s="190" t="s">
         <v>88</v>
       </c>
-      <c r="K16" s="105"/>
-      <c r="L16" s="102" t="s">
+      <c r="K16" s="190"/>
+      <c r="L16" s="191" t="s">
         <v>89</v>
       </c>
       <c r="M16" s="104"/>
@@ -3147,7 +3198,7 @@
         <v>34</v>
       </c>
       <c r="G18" s="78"/>
-      <c r="H18" s="106" t="s">
+      <c r="H18" s="105" t="s">
         <v>96</v>
       </c>
       <c r="I18" s="102"/>
@@ -3167,22 +3218,22 @@
         <v>115</v>
       </c>
       <c r="C19" s="86"/>
-      <c r="D19" s="140" t="s">
+      <c r="D19" s="192" t="s">
         <v>119</v>
       </c>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
+      <c r="E19" s="192"/>
+      <c r="F19" s="192"/>
       <c r="G19" s="98"/>
       <c r="H19" s="87" t="s">
         <v>117</v>
       </c>
       <c r="I19" s="101"/>
-      <c r="J19" s="140" t="s">
+      <c r="J19" s="192" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="140"/>
-      <c r="L19" s="140"/>
-      <c r="M19" s="141"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
+      <c r="M19" s="193"/>
       <c r="N19" s="21"/>
     </row>
     <row r="20" spans="1:14" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
@@ -3191,28 +3242,28 @@
         <v>116</v>
       </c>
       <c r="C20" s="96"/>
-      <c r="D20" s="140"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="140"/>
+      <c r="D20" s="192"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
       <c r="G20" s="98"/>
       <c r="H20" s="6" t="s">
         <v>118</v>
       </c>
       <c r="I20" s="78"/>
-      <c r="J20" s="140"/>
-      <c r="K20" s="140"/>
-      <c r="L20" s="140"/>
-      <c r="M20" s="141"/>
+      <c r="J20" s="192"/>
+      <c r="K20" s="192"/>
+      <c r="L20" s="192"/>
+      <c r="M20" s="193"/>
       <c r="N20" s="21"/>
     </row>
     <row r="21" spans="1:14" s="56" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="76"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
       <c r="G21" s="75"/>
-      <c r="H21" s="123"/>
+      <c r="H21" s="122"/>
       <c r="I21" s="74"/>
       <c r="J21" s="74"/>
       <c r="K21" s="74"/>
@@ -3224,13 +3275,13 @@
       <c r="B22" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="122"/>
-      <c r="E22" s="122"/>
-      <c r="F22" s="122"/>
-      <c r="G22" s="110"/>
+      <c r="D22" s="121"/>
+      <c r="E22" s="121"/>
+      <c r="F22" s="121"/>
+      <c r="G22" s="109"/>
       <c r="H22" s="16" t="s">
         <v>84</v>
       </c>
@@ -3240,10 +3291,10 @@
       <c r="J22" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="110" t="s">
+      <c r="K22" s="109" t="s">
         <v>81</v>
       </c>
-      <c r="L22" s="110"/>
+      <c r="L22" s="109"/>
       <c r="M22" s="17" t="s">
         <v>80</v>
       </c>
@@ -3254,12 +3305,12 @@
       <c r="B23" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="138" t="s">
+      <c r="C23" s="174" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="138"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="138"/>
+      <c r="D23" s="174"/>
+      <c r="E23" s="174"/>
+      <c r="F23" s="174"/>
       <c r="G23" s="97"/>
       <c r="H23" s="69" t="s">
         <v>77</v>
@@ -3270,10 +3321,10 @@
       <c r="J23" s="67">
         <v>14</v>
       </c>
-      <c r="K23" s="139" t="s">
+      <c r="K23" s="175" t="s">
         <v>76</v>
       </c>
-      <c r="L23" s="139"/>
+      <c r="L23" s="175"/>
       <c r="M23" s="18" t="s">
         <v>73</v>
       </c>
@@ -3281,25 +3332,25 @@
     </row>
     <row r="24" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
-      <c r="B24" s="133" t="s">
+      <c r="B24" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="134"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="134"/>
+      <c r="C24" s="170"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="170"/>
+      <c r="F24" s="170"/>
+      <c r="G24" s="170"/>
+      <c r="H24" s="170"/>
       <c r="I24" s="66" t="s">
         <v>74</v>
       </c>
       <c r="J24" s="65">
         <v>14</v>
       </c>
-      <c r="K24" s="135" t="s">
+      <c r="K24" s="171" t="s">
         <v>48</v>
       </c>
-      <c r="L24" s="135"/>
+      <c r="L24" s="171"/>
       <c r="M24" s="64" t="s">
         <v>73</v>
       </c>
@@ -3519,13 +3570,13 @@
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="14"/>
-      <c r="I38" s="107" t="s">
+      <c r="I38" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="J38" s="108"/>
-      <c r="K38" s="108"/>
-      <c r="L38" s="108"/>
-      <c r="M38" s="109"/>
+      <c r="J38" s="107"/>
+      <c r="K38" s="107"/>
+      <c r="L38" s="107"/>
+      <c r="M38" s="108"/>
       <c r="N38" s="21"/>
     </row>
     <row r="39" spans="1:14" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>